<commit_message>
update tester template for infiltration units change
</commit_message>
<xml_diff>
--- a/tests/data/template_tester_v3.xlsx
+++ b/tests/data/template_tester_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daryaguettler/MIT Dropbox/Darya Guettler/Research/epinterface/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381B4178-82CB-A245-92BF-C2C98E4547B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A2F1F2-24F8-674A-AF78-838BA271467E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16680" tabRatio="926" firstSheet="15" activeTab="23" xr2:uid="{46D55ACF-0183-F346-B7C2-C9B3BC712B05}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16680" tabRatio="926" firstSheet="11" activeTab="23" xr2:uid="{46D55ACF-0183-F346-B7C2-C9B3BC712B05}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3484" uniqueCount="929">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3485" uniqueCount="930">
   <si>
     <t>Name</t>
   </si>
@@ -2915,9 +2915,6 @@
     <t>Water_temperature_inlet</t>
   </si>
   <si>
-    <t>ACH</t>
-  </si>
-  <si>
     <t>VisibleAbsorptance</t>
   </si>
   <si>
@@ -2973,6 +2970,12 @@
   </si>
   <si>
     <t>GroundWall</t>
+  </si>
+  <si>
+    <t>Flow per exterior surface area</t>
+  </si>
+  <si>
+    <t>AirChanges/Hour</t>
   </si>
 </sst>
 </file>
@@ -9801,7 +9804,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11820,16 +11823,16 @@
         <v>3</v>
       </c>
       <c r="E2" s="104" t="s">
+        <v>910</v>
+      </c>
+      <c r="F2" s="104" t="s">
+        <v>909</v>
+      </c>
+      <c r="G2" s="104" t="s">
         <v>911</v>
       </c>
-      <c r="F2" s="104" t="s">
-        <v>910</v>
-      </c>
-      <c r="G2" s="104" t="s">
-        <v>912</v>
-      </c>
       <c r="H2" s="104" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="I2" s="79" t="s">
         <v>1</v>
@@ -29006,7 +29009,7 @@
         <v>632</v>
       </c>
       <c r="F2" s="85" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="G2" s="59" t="s">
         <v>362</v>
@@ -30196,7 +30199,7 @@
     </row>
     <row r="18" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="B18" t="s">
         <v>339</v>
@@ -30262,7 +30265,7 @@
     </row>
     <row r="19" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="B19" t="s">
         <v>343</v>
@@ -30332,7 +30335,7 @@
     </row>
     <row r="20" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="B20" t="s">
         <v>350</v>
@@ -30402,7 +30405,7 @@
     </row>
     <row r="21" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="B21" t="s">
         <v>353</v>
@@ -30465,7 +30468,7 @@
     </row>
     <row r="22" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="B22" t="s">
         <v>355</v>
@@ -30531,7 +30534,7 @@
     </row>
     <row r="23" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="B23" t="s">
         <v>538</v>
@@ -30589,7 +30592,7 @@
     </row>
     <row r="24" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="B24" t="s">
         <v>538</v>
@@ -34404,11 +34407,11 @@
   </sheetPr>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="111" workbookViewId="0">
       <pane xSplit="12" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -34437,7 +34440,9 @@
       <c r="C1" s="70" t="s">
         <v>762</v>
       </c>
-      <c r="D1" s="70"/>
+      <c r="D1" s="70" t="s">
+        <v>928</v>
+      </c>
       <c r="E1" s="70"/>
       <c r="F1" s="70"/>
       <c r="G1" s="126" t="s">
@@ -34464,10 +34469,10 @@
         <v>888</v>
       </c>
       <c r="E2" s="43" t="s">
+        <v>924</v>
+      </c>
+      <c r="F2" s="43" t="s">
         <v>925</v>
-      </c>
-      <c r="F2" s="43" t="s">
-        <v>926</v>
       </c>
       <c r="G2" s="43" t="s">
         <v>339</v>
@@ -34479,16 +34484,16 @@
         <v>343</v>
       </c>
       <c r="J2" s="43" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="K2" s="43" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="L2" s="43" t="s">
         <v>353</v>
       </c>
       <c r="M2" s="45" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="51" x14ac:dyDescent="0.2">
@@ -34535,7 +34540,7 @@
         <v>0.6</v>
       </c>
       <c r="D4" t="s">
-        <v>909</v>
+        <v>929</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -35022,103 +35027,103 @@
       </c>
       <c r="C4">
         <f ca="1">RANDBETWEEN(0,100)/100</f>
-        <v>0.85</v>
+        <v>0.75</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:AA4" ca="1" si="0">RANDBETWEEN(0,100)/100</f>
-        <v>0.91</v>
+        <v>0.37</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.52</v>
+        <v>0.7</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.77</v>
+        <v>0.86</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.97</v>
+        <v>0.18</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.6</v>
+        <v>0.13</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85</v>
+        <v>0.74</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.2</v>
+        <v>0.88</v>
       </c>
       <c r="L4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.38</v>
+        <v>0.32</v>
       </c>
       <c r="M4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.56000000000000005</v>
+        <v>0.25</v>
       </c>
       <c r="N4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="O4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.39</v>
+        <v>0.64</v>
       </c>
       <c r="P4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.84</v>
+        <v>0.44</v>
       </c>
       <c r="Q4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85</v>
+        <v>0</v>
       </c>
       <c r="R4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.14000000000000001</v>
+        <v>0.47</v>
       </c>
       <c r="S4">
         <f ca="1">RANDBETWEEN(0,100)/100</f>
-        <v>0.22</v>
+        <v>0.26</v>
       </c>
       <c r="T4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.31</v>
+        <v>0.65</v>
       </c>
       <c r="U4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.71</v>
+        <v>0.83</v>
       </c>
       <c r="V4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.64</v>
+        <v>0.03</v>
       </c>
       <c r="W4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.38</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.28000000000000003</v>
+        <v>0.48</v>
       </c>
       <c r="Y4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16</v>
+        <v>0.69</v>
       </c>
       <c r="Z4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.3</v>
+        <v>0.01</v>
       </c>
       <c r="AA4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.38</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
@@ -39694,7 +39699,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -39705,7 +39710,7 @@
         <v>765</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>766</v>

</xml_diff>

<commit_message>
update validation for lighting controls
</commit_message>
<xml_diff>
--- a/tests/data/template_tester_v3.xlsx
+++ b/tests/data/template_tester_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daryaguettler/MIT Dropbox/Darya Guettler/Research/epinterface/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A2F1F2-24F8-674A-AF78-838BA271467E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC480839-5FB8-B449-A5CC-2101274B7039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16680" tabRatio="926" firstSheet="11" activeTab="23" xr2:uid="{46D55ACF-0183-F346-B7C2-C9B3BC712B05}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16680" tabRatio="926" firstSheet="3" activeTab="8" xr2:uid="{46D55ACF-0183-F346-B7C2-C9B3BC712B05}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -2867,9 +2867,6 @@
     <t>DimmingType</t>
   </si>
   <si>
-    <t>NoDimming</t>
-  </si>
-  <si>
     <t>No_system</t>
   </si>
   <si>
@@ -2976,6 +2973,9 @@
   </si>
   <si>
     <t>AirChanges/Hour</t>
+  </si>
+  <si>
+    <t>Off</t>
   </si>
 </sst>
 </file>
@@ -6256,7 +6256,7 @@
         <v>801</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -6273,7 +6273,7 @@
         <v>801</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -6290,7 +6290,7 @@
         <v>801</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -6307,7 +6307,7 @@
         <v>801</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -6591,7 +6591,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6663,7 +6663,7 @@
         <v>847</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -6689,7 +6689,7 @@
         <v>847</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
   </sheetData>
@@ -6783,7 +6783,7 @@
         <v>691</v>
       </c>
       <c r="C2" s="54" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="D2" s="54" t="s">
         <v>608</v>
@@ -7147,7 +7147,7 @@
         <v>774</v>
       </c>
       <c r="F2" s="51" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -8058,7 +8058,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="50" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="C2" s="51" t="s">
         <v>574</v>
@@ -8070,10 +8070,10 @@
         <v>573</v>
       </c>
       <c r="F2" s="50" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="G2" s="50" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="H2" s="50" t="s">
         <v>590</v>
@@ -8108,13 +8108,13 @@
         <v>801</v>
       </c>
       <c r="H3" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="I3" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="J3" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -8140,18 +8140,18 @@
         <v>801</v>
       </c>
       <c r="H4" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="I4" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="J4" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="B5">
         <v>0.7</v>
@@ -8166,24 +8166,24 @@
         <v>589</v>
       </c>
       <c r="F5" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="G5" t="s">
         <v>801</v>
       </c>
       <c r="H5" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="I5" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="J5" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="B6">
         <v>0.7</v>
@@ -8204,13 +8204,13 @@
         <v>801</v>
       </c>
       <c r="H6" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="I6" t="s">
         <v>757</v>
       </c>
       <c r="J6" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -9666,10 +9666,10 @@
         <v>393</v>
       </c>
       <c r="C2" s="104" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D2" s="104" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="E2" s="104" t="s">
         <v>694</v>
@@ -9740,7 +9740,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="B6" t="s">
         <v>537</v>
@@ -9850,7 +9850,7 @@
     </row>
     <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="B3" t="s">
         <v>882</v>
@@ -9859,7 +9859,7 @@
         <v>890</v>
       </c>
       <c r="D3" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="E3" s="30" t="s">
         <v>583</v>
@@ -9867,7 +9867,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="B4" t="s">
         <v>858</v>
@@ -9876,10 +9876,10 @@
         <v>858</v>
       </c>
       <c r="D4" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
   </sheetData>
@@ -11823,16 +11823,16 @@
         <v>3</v>
       </c>
       <c r="E2" s="104" t="s">
+        <v>909</v>
+      </c>
+      <c r="F2" s="104" t="s">
+        <v>908</v>
+      </c>
+      <c r="G2" s="104" t="s">
         <v>910</v>
       </c>
-      <c r="F2" s="104" t="s">
-        <v>909</v>
-      </c>
-      <c r="G2" s="104" t="s">
-        <v>911</v>
-      </c>
       <c r="H2" s="104" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="I2" s="79" t="s">
         <v>1</v>
@@ -29009,7 +29009,7 @@
         <v>632</v>
       </c>
       <c r="F2" s="85" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="G2" s="59" t="s">
         <v>362</v>
@@ -30199,7 +30199,7 @@
     </row>
     <row r="18" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="B18" t="s">
         <v>339</v>
@@ -30265,7 +30265,7 @@
     </row>
     <row r="19" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="B19" t="s">
         <v>343</v>
@@ -30335,7 +30335,7 @@
     </row>
     <row r="20" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="B20" t="s">
         <v>350</v>
@@ -30405,7 +30405,7 @@
     </row>
     <row r="21" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="B21" t="s">
         <v>353</v>
@@ -30468,7 +30468,7 @@
     </row>
     <row r="22" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="B22" t="s">
         <v>355</v>
@@ -30534,7 +30534,7 @@
     </row>
     <row r="23" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="B23" t="s">
         <v>538</v>
@@ -30592,7 +30592,7 @@
     </row>
     <row r="24" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="B24" t="s">
         <v>538</v>
@@ -34407,11 +34407,11 @@
   </sheetPr>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="111" workbookViewId="0">
+    <sheetView zoomScale="111" zoomScaleNormal="111" workbookViewId="0">
       <pane xSplit="12" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -34441,7 +34441,7 @@
         <v>762</v>
       </c>
       <c r="D1" s="70" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="E1" s="70"/>
       <c r="F1" s="70"/>
@@ -34469,10 +34469,10 @@
         <v>888</v>
       </c>
       <c r="E2" s="43" t="s">
+        <v>923</v>
+      </c>
+      <c r="F2" s="43" t="s">
         <v>924</v>
-      </c>
-      <c r="F2" s="43" t="s">
-        <v>925</v>
       </c>
       <c r="G2" s="43" t="s">
         <v>339</v>
@@ -34484,16 +34484,16 @@
         <v>343</v>
       </c>
       <c r="J2" s="43" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="K2" s="43" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="L2" s="43" t="s">
         <v>353</v>
       </c>
       <c r="M2" s="45" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="51" x14ac:dyDescent="0.2">
@@ -34540,7 +34540,7 @@
         <v>0.6</v>
       </c>
       <c r="D4" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -34807,7 +34807,7 @@
   <dimension ref="A1:AA36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -35027,103 +35027,103 @@
       </c>
       <c r="C4">
         <f ca="1">RANDBETWEEN(0,100)/100</f>
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:AA4" ca="1" si="0">RANDBETWEEN(0,100)/100</f>
-        <v>0.37</v>
+        <v>0.3</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.7</v>
+        <v>0.52</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.86</v>
+        <v>0.19</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18</v>
+        <v>0.2</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.13</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.74</v>
+        <v>0.65</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.88</v>
+        <v>0.83</v>
       </c>
       <c r="L4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.32</v>
+        <v>0.79</v>
       </c>
       <c r="M4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.25</v>
+        <v>0.7</v>
       </c>
       <c r="N4">
         <f t="shared" ca="1" si="0"/>
-        <v>7.0000000000000007E-2</v>
+        <v>0.74</v>
       </c>
       <c r="O4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.64</v>
+        <v>0.52</v>
       </c>
       <c r="P4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.44</v>
+        <v>0.91</v>
       </c>
       <c r="Q4">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>0.84</v>
       </c>
       <c r="R4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.47</v>
+        <v>0.63</v>
       </c>
       <c r="S4">
         <f ca="1">RANDBETWEEN(0,100)/100</f>
-        <v>0.26</v>
+        <v>0.46</v>
       </c>
       <c r="T4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.65</v>
+        <v>0.62</v>
       </c>
       <c r="U4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.83</v>
+        <v>0.42</v>
       </c>
       <c r="V4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
       <c r="W4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.55000000000000004</v>
+        <v>0.33</v>
       </c>
       <c r="X4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.48</v>
+        <v>0.04</v>
       </c>
       <c r="Y4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.69</v>
+        <v>0.68</v>
       </c>
       <c r="Z4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.01</v>
+        <v>0.36</v>
       </c>
       <c r="AA4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.44</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
@@ -35680,8 +35680,8 @@
   </sheetPr>
   <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -39644,10 +39644,10 @@
         <v>605</v>
       </c>
       <c r="L5" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="M5" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -39699,7 +39699,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -39710,7 +39710,7 @@
         <v>765</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>766</v>
@@ -41769,8 +41769,8 @@
   </sheetPr>
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -41819,7 +41819,7 @@
         <v>5.76</v>
       </c>
       <c r="C3" t="s">
-        <v>893</v>
+        <v>929</v>
       </c>
       <c r="D3" t="s">
         <v>801</v>
@@ -41836,7 +41836,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="C4" t="s">
-        <v>893</v>
+        <v>929</v>
       </c>
       <c r="D4" t="s">
         <v>801</v>
@@ -41853,7 +41853,7 @@
         <v>2.7</v>
       </c>
       <c r="C5" t="s">
-        <v>893</v>
+        <v>929</v>
       </c>
       <c r="D5" t="s">
         <v>801</v>
@@ -41870,7 +41870,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="C6" t="s">
-        <v>893</v>
+        <v>929</v>
       </c>
       <c r="D6" t="s">
         <v>801</v>
@@ -42140,6 +42140,11 @@
       <formula>LEN(TRIM(D7))=0</formula>
     </cfRule>
   </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C6" xr:uid="{6D31588D-7A28-8D4F-98B8-250BC1772AE4}">
+      <formula1>"Stepped, Continuous, Off"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">

</xml_diff>

<commit_message>
update tester to include HeatingAndCooling option
</commit_message>
<xml_diff>
--- a/tests/data/template_tester_v3.xlsx
+++ b/tests/data/template_tester_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daryaguettler/MIT Dropbox/Darya Guettler/Research/epinterface/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC480839-5FB8-B449-A5CC-2101274B7039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756CBBB8-B674-804B-8086-8B694FBDD75F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16680" tabRatio="926" firstSheet="3" activeTab="8" xr2:uid="{46D55ACF-0183-F346-B7C2-C9B3BC712B05}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16680" tabRatio="926" firstSheet="10" activeTab="14" xr2:uid="{46D55ACF-0183-F346-B7C2-C9B3BC712B05}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3485" uniqueCount="930">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3486" uniqueCount="931">
   <si>
     <t>Name</t>
   </si>
@@ -2976,6 +2976,9 @@
   </si>
   <si>
     <t>Off</t>
+  </si>
+  <si>
+    <t>HeatingAndCooling</t>
   </si>
 </sst>
 </file>
@@ -6756,7 +6759,7 @@
   <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7271,8 +7274,8 @@
   </sheetPr>
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7533,7 +7536,7 @@
         <v>857</v>
       </c>
       <c r="B12" t="s">
-        <v>458</v>
+        <v>930</v>
       </c>
       <c r="C12" t="s">
         <v>537</v>
@@ -7557,7 +7560,7 @@
         <v>858</v>
       </c>
       <c r="B13" t="s">
-        <v>458</v>
+        <v>930</v>
       </c>
       <c r="C13" t="s">
         <v>537</v>
@@ -9804,7 +9807,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -35027,103 +35030,103 @@
       </c>
       <c r="C4">
         <f ca="1">RANDBETWEEN(0,100)/100</f>
-        <v>0.25</v>
+        <v>0.63</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:AA4" ca="1" si="0">RANDBETWEEN(0,100)/100</f>
-        <v>0.3</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.52</v>
+        <v>0.47</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.27</v>
+        <v>0.03</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.19</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.56999999999999995</v>
+        <v>0.99</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.65</v>
+        <v>0.94</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.83</v>
+        <v>1</v>
       </c>
       <c r="L4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.79</v>
+        <v>0.47</v>
       </c>
       <c r="M4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.7</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="N4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.74</v>
+        <v>0.93</v>
       </c>
       <c r="O4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.52</v>
+        <v>0.03</v>
       </c>
       <c r="P4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.91</v>
+        <v>0.73</v>
       </c>
       <c r="Q4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.84</v>
+        <v>0.24</v>
       </c>
       <c r="R4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.63</v>
+        <v>0.32</v>
       </c>
       <c r="S4">
         <f ca="1">RANDBETWEEN(0,100)/100</f>
-        <v>0.46</v>
+        <v>0.72</v>
       </c>
       <c r="T4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.62</v>
+        <v>0.98</v>
       </c>
       <c r="U4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.42</v>
+        <v>0.94</v>
       </c>
       <c r="V4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1</v>
+        <v>0.79</v>
       </c>
       <c r="W4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.33</v>
+        <v>0.85</v>
       </c>
       <c r="X4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.04</v>
+        <v>0.49</v>
       </c>
       <c r="Y4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.68</v>
+        <v>0.84</v>
       </c>
       <c r="Z4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.36</v>
+        <v>0.95</v>
       </c>
       <c r="AA4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.62</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
@@ -39493,7 +39496,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -39636,6 +39639,9 @@
       </c>
       <c r="F5" t="s">
         <v>592</v>
+      </c>
+      <c r="G5" t="s">
+        <v>930</v>
       </c>
       <c r="I5" t="s">
         <v>595</v>
@@ -41769,8 +41775,8 @@
   </sheetPr>
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update ventilation to include relevant TechTypes
</commit_message>
<xml_diff>
--- a/tests/data/template_tester_v3.xlsx
+++ b/tests/data/template_tester_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daryaguettler/MIT Dropbox/Darya Guettler/Research/epinterface/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756CBBB8-B674-804B-8086-8B694FBDD75F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92999D90-1F3E-074C-86B9-37E6313CBA37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16680" tabRatio="926" firstSheet="10" activeTab="14" xr2:uid="{46D55ACF-0183-F346-B7C2-C9B3BC712B05}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16680" tabRatio="926" firstSheet="11" activeTab="15" xr2:uid="{46D55ACF-0183-F346-B7C2-C9B3BC712B05}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3486" uniqueCount="931">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3492" uniqueCount="933">
   <si>
     <t>Name</t>
   </si>
@@ -2900,9 +2900,6 @@
     <t>Tech_type</t>
   </si>
   <si>
-    <t>Supply_ventilation</t>
-  </si>
-  <si>
     <t>Window_schedule</t>
   </si>
   <si>
@@ -2979,6 +2976,15 @@
   </si>
   <si>
     <t>HeatingAndCooling</t>
+  </si>
+  <si>
+    <t>VentilationTechType</t>
+  </si>
+  <si>
+    <t>ERV</t>
+  </si>
+  <si>
+    <t>Custom</t>
   </si>
 </sst>
 </file>
@@ -6741,7 +6747,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2D650E4A-B813-4110-AEE8-5EE5CA86EC4F}">
           <x14:formula1>
-            <xm:f>HVAC_options!$K$3:$K$14</xm:f>
+            <xm:f>HVAC_options!$L$3:$L$14</xm:f>
           </x14:formula1>
           <xm:sqref>B3:B46</xm:sqref>
         </x14:dataValidation>
@@ -7274,8 +7280,8 @@
   </sheetPr>
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7536,7 +7542,7 @@
         <v>857</v>
       </c>
       <c r="B12" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="C12" t="s">
         <v>537</v>
@@ -7560,7 +7566,7 @@
         <v>858</v>
       </c>
       <c r="B13" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="C13" t="s">
         <v>537</v>
@@ -8006,13 +8012,13 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{611028E8-488F-44DF-9A4F-6910180A9024}">
           <x14:formula1>
-            <xm:f>HVAC_options!$G$3:$G$7</xm:f>
+            <xm:f>HVAC_options!$H$3:$H$7</xm:f>
           </x14:formula1>
           <xm:sqref>B3:B43</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{16062F8E-C39B-4811-9C9A-80842E3D663F}">
           <x14:formula1>
-            <xm:f>HVAC_options!$I$3:$I$13</xm:f>
+            <xm:f>HVAC_options!$J$3:$J$13</xm:f>
           </x14:formula1>
           <xm:sqref>D40:D49 C3:C49</xm:sqref>
         </x14:dataValidation>
@@ -8029,8 +8035,8 @@
   </sheetPr>
   <dimension ref="A1:J208"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8076,7 +8082,7 @@
         <v>903</v>
       </c>
       <c r="G2" s="50" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="H2" s="50" t="s">
         <v>590</v>
@@ -8105,7 +8111,7 @@
         <v>588</v>
       </c>
       <c r="F3" t="s">
-        <v>588</v>
+        <v>593</v>
       </c>
       <c r="G3" t="s">
         <v>801</v>
@@ -8137,7 +8143,7 @@
         <v>588</v>
       </c>
       <c r="F4" t="s">
-        <v>588</v>
+        <v>593</v>
       </c>
       <c r="G4" t="s">
         <v>801</v>
@@ -8169,7 +8175,7 @@
         <v>589</v>
       </c>
       <c r="F5" t="s">
-        <v>904</v>
+        <v>593</v>
       </c>
       <c r="G5" t="s">
         <v>801</v>
@@ -9230,7 +9236,7 @@
   <mergeCells count="1">
     <mergeCell ref="C1:J1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A3:F3 E4:F6 H4:I124 E7:J121 A4:C121 D4:D208">
+  <conditionalFormatting sqref="A3:F3 H4:I124 E7:J121 A4:C121 D4:D208 E4:F6 F3:F6">
     <cfRule type="containsBlanks" dxfId="25" priority="4">
       <formula>LEN(TRIM(A3))=0</formula>
     </cfRule>
@@ -9248,28 +9254,28 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EB7C07FE-48F2-46EF-BFBD-F1C4D94A1CD0}">
           <x14:formula1>
-            <xm:f>HVAC_options!$E$3:$E$7</xm:f>
+            <xm:f>HVAC_options!$F$3:$F$7</xm:f>
           </x14:formula1>
-          <xm:sqref>E3:E50 F7:G50 F3:F4</xm:sqref>
+          <xm:sqref>E3:E50 F7:G50</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{75727552-93B4-4D7E-835C-6E2046BF9729}">
           <x14:formula1>
-            <xm:f>HVAC_options!$F$3:$F$11</xm:f>
+            <xm:f>HVAC_options!$G$3:$G$11</xm:f>
           </x14:formula1>
           <xm:sqref>J7:J53</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{772049FA-CA8D-924A-9ACC-0C7311E6D2D2}">
           <x14:formula1>
-            <xm:f>HVAC_options!$L$3:$L$7</xm:f>
+            <xm:f>HVAC_options!$M$3:$M$7</xm:f>
           </x14:formula1>
           <xm:sqref>H3:H124</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F86E37D1-7884-434A-AA2F-495663D0E5C5}">
           <x14:formula1>
-            <xm:f>HVAC_options!$M$3:$M$7</xm:f>
+            <xm:f>HVAC_options!$N$3:$N$7</xm:f>
           </x14:formula1>
           <xm:sqref>J3:J6 I3:I124</xm:sqref>
         </x14:dataValidation>
@@ -9278,6 +9284,12 @@
             <xm:f>Schedule_choices!$C$2:$C$44</xm:f>
           </x14:formula1>
           <xm:sqref>G3:G6</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{68CE51BA-1EE5-3849-A6B0-F6D8341EF639}">
+          <x14:formula1>
+            <xm:f>HVAC_options!$E$3:$E$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>F3:F6</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -9669,10 +9681,10 @@
         <v>393</v>
       </c>
       <c r="C2" s="104" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="D2" s="104" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="E2" s="104" t="s">
         <v>694</v>
@@ -11826,16 +11838,16 @@
         <v>3</v>
       </c>
       <c r="E2" s="104" t="s">
+        <v>908</v>
+      </c>
+      <c r="F2" s="104" t="s">
+        <v>907</v>
+      </c>
+      <c r="G2" s="104" t="s">
         <v>909</v>
       </c>
-      <c r="F2" s="104" t="s">
-        <v>908</v>
-      </c>
-      <c r="G2" s="104" t="s">
-        <v>910</v>
-      </c>
       <c r="H2" s="104" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="I2" s="79" t="s">
         <v>1</v>
@@ -29012,7 +29024,7 @@
         <v>632</v>
       </c>
       <c r="F2" s="85" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="G2" s="59" t="s">
         <v>362</v>
@@ -30202,7 +30214,7 @@
     </row>
     <row r="18" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="B18" t="s">
         <v>339</v>
@@ -30268,7 +30280,7 @@
     </row>
     <row r="19" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="B19" t="s">
         <v>343</v>
@@ -30338,7 +30350,7 @@
     </row>
     <row r="20" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="B20" t="s">
         <v>350</v>
@@ -30408,7 +30420,7 @@
     </row>
     <row r="21" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="B21" t="s">
         <v>353</v>
@@ -30471,7 +30483,7 @@
     </row>
     <row r="22" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="B22" t="s">
         <v>355</v>
@@ -30537,7 +30549,7 @@
     </row>
     <row r="23" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="B23" t="s">
         <v>538</v>
@@ -30595,7 +30607,7 @@
     </row>
     <row r="24" spans="1:84" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="B24" t="s">
         <v>538</v>
@@ -34444,7 +34456,7 @@
         <v>762</v>
       </c>
       <c r="D1" s="70" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="E1" s="70"/>
       <c r="F1" s="70"/>
@@ -34472,10 +34484,10 @@
         <v>888</v>
       </c>
       <c r="E2" s="43" t="s">
+        <v>922</v>
+      </c>
+      <c r="F2" s="43" t="s">
         <v>923</v>
-      </c>
-      <c r="F2" s="43" t="s">
-        <v>924</v>
       </c>
       <c r="G2" s="43" t="s">
         <v>339</v>
@@ -34487,16 +34499,16 @@
         <v>343</v>
       </c>
       <c r="J2" s="43" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="K2" s="43" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="L2" s="43" t="s">
         <v>353</v>
       </c>
       <c r="M2" s="45" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="51" x14ac:dyDescent="0.2">
@@ -34543,7 +34555,7 @@
         <v>0.6</v>
       </c>
       <c r="D4" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -35030,103 +35042,103 @@
       </c>
       <c r="C4">
         <f ca="1">RANDBETWEEN(0,100)/100</f>
-        <v>0.63</v>
+        <v>0.05</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:AA4" ca="1" si="0">RANDBETWEEN(0,100)/100</f>
-        <v>0.57999999999999996</v>
+        <v>0.99</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.47</v>
+        <v>0.63</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.03</v>
+        <v>0.95</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>7.0000000000000007E-2</v>
+        <v>0.78</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.7</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.99</v>
+        <v>0.64</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.94</v>
+        <v>0.7</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="L4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.47</v>
+        <v>0.27</v>
       </c>
       <c r="M4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.28000000000000003</v>
+        <v>0.51</v>
       </c>
       <c r="N4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.93</v>
+        <v>0.86</v>
       </c>
       <c r="O4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.03</v>
+        <v>0.67</v>
       </c>
       <c r="P4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.73</v>
+        <v>0.34</v>
       </c>
       <c r="Q4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.24</v>
+        <v>0.04</v>
       </c>
       <c r="R4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.32</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="S4">
         <f ca="1">RANDBETWEEN(0,100)/100</f>
-        <v>0.72</v>
+        <v>0.94</v>
       </c>
       <c r="T4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.98</v>
+        <v>0.87</v>
       </c>
       <c r="U4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.94</v>
+        <v>0.85</v>
       </c>
       <c r="V4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.79</v>
+        <v>0.2</v>
       </c>
       <c r="W4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85</v>
+        <v>0.62</v>
       </c>
       <c r="X4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.49</v>
+        <v>0.43</v>
       </c>
       <c r="Y4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.84</v>
+        <v>0.71</v>
       </c>
       <c r="Z4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.95</v>
+        <v>0.91</v>
       </c>
       <c r="AA4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.31</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
@@ -39493,33 +39505,35 @@
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
     <col min="2" max="2" width="22.1640625" customWidth="1"/>
-    <col min="3" max="10" width="15.1640625" customWidth="1"/>
-    <col min="11" max="11" width="24.1640625" customWidth="1"/>
-    <col min="12" max="12" width="19.1640625" customWidth="1"/>
+    <col min="3" max="4" width="15.1640625" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+    <col min="6" max="11" width="15.1640625" customWidth="1"/>
+    <col min="12" max="12" width="24.1640625" customWidth="1"/>
+    <col min="13" max="13" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>391</v>
       </c>
       <c r="D1" t="s">
         <v>576</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="50" t="s">
         <v>393</v>
       </c>
@@ -39532,35 +39546,38 @@
       <c r="D2" s="51" t="s">
         <v>574</v>
       </c>
-      <c r="E2" s="50" t="s">
+      <c r="E2" s="51" t="s">
+        <v>930</v>
+      </c>
+      <c r="F2" s="50" t="s">
         <v>573</v>
       </c>
-      <c r="F2" s="52" t="s">
+      <c r="G2" s="52" t="s">
         <v>584</v>
       </c>
-      <c r="G2" s="50" t="s">
+      <c r="H2" s="50" t="s">
         <v>580</v>
       </c>
-      <c r="H2" s="50" t="s">
+      <c r="I2" s="50" t="s">
         <v>579</v>
       </c>
-      <c r="I2" s="51" t="s">
+      <c r="J2" s="51" t="s">
         <v>577</v>
       </c>
-      <c r="J2" s="50" t="s">
+      <c r="K2" s="50" t="s">
         <v>578</v>
       </c>
-      <c r="K2" s="79" t="s">
+      <c r="L2" s="79" t="s">
         <v>572</v>
       </c>
-      <c r="L2" s="79" t="s">
+      <c r="M2" s="79" t="s">
         <v>590</v>
       </c>
-      <c r="M2" s="79" t="s">
+      <c r="N2" s="79" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>582</v>
       </c>
@@ -39571,31 +39588,34 @@
         <v>598</v>
       </c>
       <c r="E3" t="s">
+        <v>931</v>
+      </c>
+      <c r="F3" t="s">
         <v>588</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>590</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>458</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>594</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>582</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>606</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>758</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>757</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>586</v>
       </c>
@@ -39606,68 +39626,82 @@
         <v>597</v>
       </c>
       <c r="E4" t="s">
+        <v>591</v>
+      </c>
+      <c r="F4" t="s">
         <v>589</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>591</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>575</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>581</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>586</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>604</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>759</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>760</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>537</v>
       </c>
       <c r="D5" t="s">
         <v>599</v>
       </c>
-      <c r="F5" t="s">
+      <c r="E5" t="s">
+        <v>763</v>
+      </c>
+      <c r="G5" t="s">
         <v>592</v>
       </c>
-      <c r="G5" t="s">
-        <v>930</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="H5" t="s">
+        <v>929</v>
+      </c>
+      <c r="J5" t="s">
         <v>595</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>605</v>
-      </c>
-      <c r="L5" t="s">
-        <v>893</v>
       </c>
       <c r="M5" t="s">
         <v>893</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N5" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>761</v>
       </c>
       <c r="D6" t="s">
         <v>600</v>
       </c>
-      <c r="F6" t="s">
+      <c r="E6" t="s">
         <v>593</v>
       </c>
-      <c r="I6" t="s">
+      <c r="G6" t="s">
+        <v>593</v>
+      </c>
+      <c r="J6" t="s">
         <v>537</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>932</v>
       </c>
     </row>
   </sheetData>
@@ -39705,7 +39739,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -39716,7 +39750,7 @@
         <v>765</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>766</v>
@@ -41825,7 +41859,7 @@
         <v>5.76</v>
       </c>
       <c r="C3" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="D3" t="s">
         <v>801</v>
@@ -41842,7 +41876,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="C4" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="D4" t="s">
         <v>801</v>
@@ -41859,7 +41893,7 @@
         <v>2.7</v>
       </c>
       <c r="C5" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="D5" t="s">
         <v>801</v>
@@ -41876,7 +41910,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="C6" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="D6" t="s">
         <v>801</v>

</xml_diff>

<commit_message>
update ventilation to include new TechTypes NoMechanicalVentilation
</commit_message>
<xml_diff>
--- a/tests/data/template_tester_v3.xlsx
+++ b/tests/data/template_tester_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daryaguettler/MIT Dropbox/Darya Guettler/Research/epinterface/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92999D90-1F3E-074C-86B9-37E6313CBA37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4046714-5962-BA45-984D-A75349B884D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16680" tabRatio="926" firstSheet="11" activeTab="15" xr2:uid="{46D55ACF-0183-F346-B7C2-C9B3BC712B05}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16680" tabRatio="926" firstSheet="10" activeTab="15" xr2:uid="{46D55ACF-0183-F346-B7C2-C9B3BC712B05}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -101,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3492" uniqueCount="933">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3492" uniqueCount="934">
   <si>
     <t>Name</t>
   </si>
@@ -2985,6 +2985,9 @@
   </si>
   <si>
     <t>Custom</t>
+  </si>
+  <si>
+    <t>NoMechanicalVentilation</t>
   </si>
 </sst>
 </file>
@@ -8036,7 +8039,7 @@
   <dimension ref="A1:J208"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F3" sqref="F3:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8111,7 +8114,7 @@
         <v>588</v>
       </c>
       <c r="F3" t="s">
-        <v>593</v>
+        <v>933</v>
       </c>
       <c r="G3" t="s">
         <v>801</v>
@@ -8143,7 +8146,7 @@
         <v>588</v>
       </c>
       <c r="F4" t="s">
-        <v>593</v>
+        <v>933</v>
       </c>
       <c r="G4" t="s">
         <v>801</v>
@@ -8175,7 +8178,7 @@
         <v>589</v>
       </c>
       <c r="F5" t="s">
-        <v>593</v>
+        <v>933</v>
       </c>
       <c r="G5" t="s">
         <v>801</v>
@@ -35042,103 +35045,103 @@
       </c>
       <c r="C4">
         <f ca="1">RANDBETWEEN(0,100)/100</f>
-        <v>0.05</v>
+        <v>0.24</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:AA4" ca="1" si="0">RANDBETWEEN(0,100)/100</f>
-        <v>0.99</v>
+        <v>0.7</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.63</v>
+        <v>0.75</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.95</v>
+        <v>0.97</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.78</v>
+        <v>0.67</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.28999999999999998</v>
+        <v>0.98</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.64</v>
+        <v>0.69</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.7</v>
+        <v>0.31</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.28999999999999998</v>
+        <v>0.97</v>
       </c>
       <c r="L4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.27</v>
+        <v>0.03</v>
       </c>
       <c r="M4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.51</v>
+        <v>0.8</v>
       </c>
       <c r="N4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.86</v>
+        <v>0.01</v>
       </c>
       <c r="O4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.67</v>
+        <v>0.93</v>
       </c>
       <c r="P4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.34</v>
+        <v>0.03</v>
       </c>
       <c r="Q4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.04</v>
+        <v>0.21</v>
       </c>
       <c r="R4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.56000000000000005</v>
+        <v>0.38</v>
       </c>
       <c r="S4">
         <f ca="1">RANDBETWEEN(0,100)/100</f>
-        <v>0.94</v>
+        <v>0.63</v>
       </c>
       <c r="T4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.87</v>
+        <v>0.53</v>
       </c>
       <c r="U4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85</v>
+        <v>0.72</v>
       </c>
       <c r="V4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.2</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="W4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.62</v>
+        <v>0.16</v>
       </c>
       <c r="X4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.43</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="Y4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.71</v>
+        <v>0.6</v>
       </c>
       <c r="Z4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.91</v>
+        <v>0.1</v>
       </c>
       <c r="AA4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.6</v>
+        <v>0.43</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
@@ -39508,7 +39511,7 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -39690,7 +39693,7 @@
         <v>600</v>
       </c>
       <c r="E6" t="s">
-        <v>593</v>
+        <v>933</v>
       </c>
       <c r="G6" t="s">
         <v>593</v>

</xml_diff>

<commit_message>
update water temperatures checks
</commit_message>
<xml_diff>
--- a/tests/data/template_tester_v3.xlsx
+++ b/tests/data/template_tester_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daryaguettler/MIT Dropbox/Darya Guettler/Research/epinterface/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4046714-5962-BA45-984D-A75349B884D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB029D5A-1EDA-FE48-AF14-2213A06E203E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16680" tabRatio="926" firstSheet="10" activeTab="15" xr2:uid="{46D55ACF-0183-F346-B7C2-C9B3BC712B05}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16680" tabRatio="926" firstSheet="9" activeTab="17" xr2:uid="{46D55ACF-0183-F346-B7C2-C9B3BC712B05}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -8038,8 +8038,8 @@
   </sheetPr>
   <dimension ref="A1:J208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F5"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9651,8 +9651,8 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9704,10 +9704,10 @@
         <v>537</v>
       </c>
       <c r="C3">
+        <v>50</v>
+      </c>
+      <c r="D3">
         <v>70</v>
-      </c>
-      <c r="D3">
-        <v>50</v>
       </c>
       <c r="E3">
         <v>0.9</v>
@@ -9724,10 +9724,10 @@
         <v>582</v>
       </c>
       <c r="C4">
+        <v>50</v>
+      </c>
+      <c r="D4">
         <v>70</v>
-      </c>
-      <c r="D4">
-        <v>50</v>
       </c>
       <c r="E4">
         <v>0.9</v>
@@ -9744,10 +9744,10 @@
         <v>586</v>
       </c>
       <c r="C5">
+        <v>50</v>
+      </c>
+      <c r="D5">
         <v>70</v>
-      </c>
-      <c r="D5">
-        <v>50</v>
       </c>
       <c r="E5">
         <v>0.9</v>
@@ -9764,10 +9764,10 @@
         <v>537</v>
       </c>
       <c r="C6">
+        <v>50</v>
+      </c>
+      <c r="D6">
         <v>70</v>
-      </c>
-      <c r="D6">
-        <v>50</v>
       </c>
       <c r="E6">
         <v>0.9</v>
@@ -35045,59 +35045,59 @@
       </c>
       <c r="C4">
         <f ca="1">RANDBETWEEN(0,100)/100</f>
-        <v>0.24</v>
+        <v>0.18</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:AA4" ca="1" si="0">RANDBETWEEN(0,100)/100</f>
-        <v>0.7</v>
+        <v>0.76</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.75</v>
+        <v>0.32</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.97</v>
+        <v>0.34</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.67</v>
+        <v>0.05</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.98</v>
+        <v>0.83</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.69</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.31</v>
+        <v>0.1</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.97</v>
+        <v>0.5</v>
       </c>
       <c r="L4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.03</v>
+        <v>1</v>
       </c>
       <c r="M4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="N4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.01</v>
+        <v>0.08</v>
       </c>
       <c r="O4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.93</v>
+        <v>0.46</v>
       </c>
       <c r="P4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.03</v>
+        <v>0.21</v>
       </c>
       <c r="Q4">
         <f t="shared" ca="1" si="0"/>
@@ -35105,43 +35105,43 @@
       </c>
       <c r="R4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.38</v>
+        <v>0.03</v>
       </c>
       <c r="S4">
         <f ca="1">RANDBETWEEN(0,100)/100</f>
-        <v>0.63</v>
+        <v>0.51</v>
       </c>
       <c r="T4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.53</v>
+        <v>0.65</v>
       </c>
       <c r="U4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.72</v>
+        <v>0.46</v>
       </c>
       <c r="V4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.28000000000000003</v>
+        <v>0.33</v>
       </c>
       <c r="W4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16</v>
+        <v>0.97</v>
       </c>
       <c r="X4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.57999999999999996</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="Y4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.6</v>
+        <v>0.37</v>
       </c>
       <c r="Z4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1</v>
+        <v>0.6</v>
       </c>
       <c r="AA4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.43</v>
+        <v>0.54</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update assemblies to meet the type requirements
</commit_message>
<xml_diff>
--- a/tests/data/template_tester_v3.xlsx
+++ b/tests/data/template_tester_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daryaguettler/MIT Dropbox/Darya Guettler/Research/epinterface/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2698BA85-7C55-DA43-B0E4-9254F8F1A656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D186E939-A355-3A4A-B989-26D1C3BF4659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16680" tabRatio="926" firstSheet="14" activeTab="21" xr2:uid="{46D55ACF-0183-F346-B7C2-C9B3BC712B05}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16680" tabRatio="926" firstSheet="14" activeTab="23" xr2:uid="{46D55ACF-0183-F346-B7C2-C9B3BC712B05}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -3856,7 +3856,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3965,9 +3965,6 @@
     <xf numFmtId="0" fontId="11" fillId="39" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="39" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -4152,7 +4149,91 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="55">
+  <dxfs count="59">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -5980,13 +6061,13 @@
         <v>839</v>
       </c>
       <c r="D3" s="26"/>
-      <c r="G3" s="105" t="s">
+      <c r="G3" s="104" t="s">
         <v>480</v>
       </c>
-      <c r="H3" s="105"/>
-      <c r="I3" s="105"/>
-      <c r="J3" s="106"/>
-      <c r="K3" s="91"/>
+      <c r="H3" s="104"/>
+      <c r="I3" s="104"/>
+      <c r="J3" s="105"/>
+      <c r="K3" s="90"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
@@ -6058,7 +6139,7 @@
       <c r="J10" s="20"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="107" t="s">
+      <c r="A11" s="106" t="s">
         <v>835</v>
       </c>
       <c r="B11" s="19" t="s">
@@ -6070,7 +6151,7 @@
       <c r="J11" s="20"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="107"/>
+      <c r="A12" s="106"/>
       <c r="B12" s="19" t="s">
         <v>404</v>
       </c>
@@ -6149,7 +6230,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="19"/>
-      <c r="G21" s="89"/>
+      <c r="G21" s="88"/>
       <c r="H21" s="17" t="s">
         <v>688</v>
       </c>
@@ -6188,7 +6269,7 @@
     <mergeCell ref="A11:A12"/>
   </mergeCells>
   <conditionalFormatting sqref="G20">
-    <cfRule type="containsBlanks" dxfId="54" priority="1">
+    <cfRule type="containsBlanks" dxfId="58" priority="1">
       <formula>LEN(TRIM(G20))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6226,14 +6307,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="79" t="s">
         <v>453</v>
       </c>
-      <c r="B1" s="101" t="s">
+      <c r="B1" s="100" t="s">
         <v>829</v>
       </c>
       <c r="C1" s="11"/>
-      <c r="D1" s="101" t="s">
+      <c r="D1" s="100" t="s">
         <v>830</v>
       </c>
     </row>
@@ -6569,12 +6650,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:D3 D4:D57 B4:C55">
-    <cfRule type="containsBlanks" dxfId="41" priority="2">
+    <cfRule type="containsBlanks" dxfId="45" priority="2">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D57">
-    <cfRule type="containsBlanks" dxfId="40" priority="1">
+    <cfRule type="containsBlanks" dxfId="44" priority="1">
       <formula>LEN(TRIM(D3))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6616,7 +6697,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="79" t="s">
         <v>453</v>
       </c>
       <c r="B1" s="67"/>
@@ -6706,30 +6787,30 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:B55">
-    <cfRule type="containsBlanks" dxfId="39" priority="5">
+    <cfRule type="containsBlanks" dxfId="43" priority="5">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:C55">
-    <cfRule type="containsBlanks" dxfId="38" priority="6">
+    <cfRule type="containsBlanks" dxfId="42" priority="6">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D55">
-    <cfRule type="containsBlanks" dxfId="37" priority="3">
+    <cfRule type="containsBlanks" dxfId="41" priority="3">
       <formula>LEN(TRIM(D3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:E55">
-    <cfRule type="containsBlanks" dxfId="36" priority="4">
+    <cfRule type="containsBlanks" dxfId="40" priority="4">
       <formula>LEN(TRIM(D3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:G55">
-    <cfRule type="containsBlanks" dxfId="35" priority="1">
+    <cfRule type="containsBlanks" dxfId="39" priority="1">
       <formula>LEN(TRIM(F3))=0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="34" priority="2">
+    <cfRule type="containsBlanks" dxfId="38" priority="2">
       <formula>LEN(TRIM(F3))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6780,12 +6861,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="79" t="s">
         <v>453</v>
       </c>
       <c r="B1" s="67"/>
       <c r="C1" s="67"/>
-      <c r="D1" s="80"/>
+      <c r="D1" s="79"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="50" t="s">
@@ -7083,17 +7164,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:D55">
-    <cfRule type="containsBlanks" dxfId="33" priority="2">
+    <cfRule type="containsBlanks" dxfId="37" priority="2">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B307:D1048576">
-    <cfRule type="containsBlanks" dxfId="32" priority="3">
+    <cfRule type="containsBlanks" dxfId="36" priority="3">
       <formula>LEN(TRIM(B307))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="containsBlanks" dxfId="31" priority="1">
+    <cfRule type="containsBlanks" dxfId="35" priority="1">
       <formula>LEN(TRIM(C3))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7131,16 +7212,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="46" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="79" t="s">
         <v>453</v>
       </c>
-      <c r="B1" s="122" t="s">
+      <c r="B1" s="121" t="s">
         <v>786</v>
       </c>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
     </row>
     <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="50" t="s">
@@ -7208,10 +7289,10 @@
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <conditionalFormatting sqref="B3:F55">
-    <cfRule type="containsBlanks" dxfId="30" priority="1">
+    <cfRule type="containsBlanks" dxfId="34" priority="1">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="29" priority="2">
+    <cfRule type="containsBlanks" dxfId="33" priority="2">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7298,7 +7379,7 @@
       <c r="A1" s="53" t="s">
         <v>453</v>
       </c>
-      <c r="B1" s="88" t="s">
+      <c r="B1" s="87" t="s">
         <v>455</v>
       </c>
       <c r="C1" s="67"/>
@@ -7307,7 +7388,7 @@
         <v>884</v>
       </c>
       <c r="F1" s="67"/>
-      <c r="G1" s="80" t="s">
+      <c r="G1" s="79" t="s">
         <v>689</v>
       </c>
     </row>
@@ -7353,7 +7434,7 @@
       <c r="F3" s="30">
         <v>0.6</v>
       </c>
-      <c r="G3" s="86">
+      <c r="G3" s="85">
         <f>E3*F3</f>
         <v>0.49199999999999994</v>
       </c>
@@ -7377,7 +7458,7 @@
       <c r="F4" s="30">
         <v>0.6</v>
       </c>
-      <c r="G4" s="86">
+      <c r="G4" s="85">
         <f t="shared" ref="G4:G57" si="0">E4*F4</f>
         <v>0.56999999999999995</v>
       </c>
@@ -7401,7 +7482,7 @@
       <c r="F5" s="30">
         <v>0.6</v>
       </c>
-      <c r="G5" s="86">
+      <c r="G5" s="85">
         <f t="shared" si="0"/>
         <v>0.48</v>
       </c>
@@ -7425,7 +7506,7 @@
       <c r="F6" s="30">
         <v>0.6</v>
       </c>
-      <c r="G6" s="86">
+      <c r="G6" s="85">
         <f t="shared" si="0"/>
         <v>0.54600000000000004</v>
       </c>
@@ -7447,7 +7528,7 @@
         <v>0.91</v>
       </c>
       <c r="F7" s="30"/>
-      <c r="G7" s="86">
+      <c r="G7" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7469,7 +7550,7 @@
         <v>0.91</v>
       </c>
       <c r="F8" s="30"/>
-      <c r="G8" s="86">
+      <c r="G8" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7491,7 +7572,7 @@
         <v>0.91</v>
       </c>
       <c r="F9" s="30"/>
-      <c r="G9" s="86">
+      <c r="G9" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7513,7 +7594,7 @@
         <v>0.91</v>
       </c>
       <c r="F10" s="30"/>
-      <c r="G10" s="86">
+      <c r="G10" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7535,7 +7616,7 @@
         <v>0.91</v>
       </c>
       <c r="F11" s="30"/>
-      <c r="G11" s="86">
+      <c r="G11" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7559,7 +7640,7 @@
       <c r="F12" s="30">
         <v>0.85</v>
       </c>
-      <c r="G12" s="86">
+      <c r="G12" s="85">
         <f t="shared" si="0"/>
         <v>3.3149999999999999</v>
       </c>
@@ -7583,7 +7664,7 @@
       <c r="F13" s="30">
         <v>0.8</v>
       </c>
-      <c r="G13" s="86">
+      <c r="G13" s="85">
         <f t="shared" si="0"/>
         <v>2.4800000000000004</v>
       </c>
@@ -7605,7 +7686,7 @@
         <v>0.91</v>
       </c>
       <c r="F14" s="30"/>
-      <c r="G14" s="86">
+      <c r="G14" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7621,7 +7702,7 @@
         <v>0.91</v>
       </c>
       <c r="F15" s="30"/>
-      <c r="G15" s="86">
+      <c r="G15" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7637,7 +7718,7 @@
         <v>0.91</v>
       </c>
       <c r="F16" s="30"/>
-      <c r="G16" s="86">
+      <c r="G16" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7661,7 +7742,7 @@
       <c r="F17" s="30">
         <v>0.8</v>
       </c>
-      <c r="G17" s="86">
+      <c r="G17" s="85">
         <f t="shared" si="0"/>
         <v>2.8000000000000003</v>
       </c>
@@ -7669,7 +7750,7 @@
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
-      <c r="G18" s="86">
+      <c r="G18" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7677,7 +7758,7 @@
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
-      <c r="G19" s="86">
+      <c r="G19" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7685,7 +7766,7 @@
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E20" s="30"/>
       <c r="F20" s="30"/>
-      <c r="G20" s="86">
+      <c r="G20" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7693,7 +7774,7 @@
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E21" s="30"/>
       <c r="F21" s="30"/>
-      <c r="G21" s="86">
+      <c r="G21" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7701,7 +7782,7 @@
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E22" s="30"/>
       <c r="F22" s="30"/>
-      <c r="G22" s="86">
+      <c r="G22" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7709,7 +7790,7 @@
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E23" s="30"/>
       <c r="F23" s="30"/>
-      <c r="G23" s="86">
+      <c r="G23" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7717,7 +7798,7 @@
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E24" s="30"/>
       <c r="F24" s="30"/>
-      <c r="G24" s="86">
+      <c r="G24" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7725,7 +7806,7 @@
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E25" s="30"/>
       <c r="F25" s="30"/>
-      <c r="G25" s="86">
+      <c r="G25" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7733,7 +7814,7 @@
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E26" s="30"/>
       <c r="F26" s="30"/>
-      <c r="G26" s="86">
+      <c r="G26" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7741,7 +7822,7 @@
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E27" s="30"/>
       <c r="F27" s="30"/>
-      <c r="G27" s="86">
+      <c r="G27" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7749,7 +7830,7 @@
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E28" s="30"/>
       <c r="F28" s="30"/>
-      <c r="G28" s="86">
+      <c r="G28" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7757,7 +7838,7 @@
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E29" s="30"/>
       <c r="F29" s="30"/>
-      <c r="G29" s="86">
+      <c r="G29" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7765,7 +7846,7 @@
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E30" s="30"/>
       <c r="F30" s="30"/>
-      <c r="G30" s="86">
+      <c r="G30" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7773,7 +7854,7 @@
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E31" s="30"/>
       <c r="F31" s="30"/>
-      <c r="G31" s="86">
+      <c r="G31" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7781,7 +7862,7 @@
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E32" s="30"/>
       <c r="F32" s="30"/>
-      <c r="G32" s="86">
+      <c r="G32" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7789,7 +7870,7 @@
     <row r="33" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E33" s="30"/>
       <c r="F33" s="30"/>
-      <c r="G33" s="86">
+      <c r="G33" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7797,7 +7878,7 @@
     <row r="34" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E34" s="30"/>
       <c r="F34" s="30"/>
-      <c r="G34" s="86">
+      <c r="G34" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7805,7 +7886,7 @@
     <row r="35" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E35" s="30"/>
       <c r="F35" s="30"/>
-      <c r="G35" s="86">
+      <c r="G35" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7813,7 +7894,7 @@
     <row r="36" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E36" s="30"/>
       <c r="F36" s="30"/>
-      <c r="G36" s="86">
+      <c r="G36" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7821,7 +7902,7 @@
     <row r="37" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E37" s="30"/>
       <c r="F37" s="30"/>
-      <c r="G37" s="86">
+      <c r="G37" s="85">
         <f>E37*F37</f>
         <v>0</v>
       </c>
@@ -7829,7 +7910,7 @@
     <row r="38" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E38" s="30"/>
       <c r="F38" s="30"/>
-      <c r="G38" s="86">
+      <c r="G38" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7837,7 +7918,7 @@
     <row r="39" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E39" s="30"/>
       <c r="F39" s="30"/>
-      <c r="G39" s="86">
+      <c r="G39" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7845,7 +7926,7 @@
     <row r="40" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E40" s="30"/>
       <c r="F40" s="30"/>
-      <c r="G40" s="86">
+      <c r="G40" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7853,7 +7934,7 @@
     <row r="41" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E41" s="30"/>
       <c r="F41" s="30"/>
-      <c r="G41" s="86">
+      <c r="G41" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7861,7 +7942,7 @@
     <row r="42" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E42" s="30"/>
       <c r="F42" s="30"/>
-      <c r="G42" s="86">
+      <c r="G42" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7869,7 +7950,7 @@
     <row r="43" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E43" s="30"/>
       <c r="F43" s="30"/>
-      <c r="G43" s="86">
+      <c r="G43" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7877,7 +7958,7 @@
     <row r="44" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E44" s="30"/>
       <c r="F44" s="30"/>
-      <c r="G44" s="86">
+      <c r="G44" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7885,7 +7966,7 @@
     <row r="45" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E45" s="30"/>
       <c r="F45" s="30"/>
-      <c r="G45" s="86">
+      <c r="G45" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7893,7 +7974,7 @@
     <row r="46" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E46" s="30"/>
       <c r="F46" s="30"/>
-      <c r="G46" s="86">
+      <c r="G46" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7901,7 +7982,7 @@
     <row r="47" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E47" s="30"/>
       <c r="F47" s="30"/>
-      <c r="G47" s="86">
+      <c r="G47" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7909,7 +7990,7 @@
     <row r="48" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E48" s="30"/>
       <c r="F48" s="30"/>
-      <c r="G48" s="86">
+      <c r="G48" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7917,7 +7998,7 @@
     <row r="49" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E49" s="30"/>
       <c r="F49" s="30"/>
-      <c r="G49" s="86">
+      <c r="G49" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7925,7 +8006,7 @@
     <row r="50" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E50" s="30"/>
       <c r="F50" s="30"/>
-      <c r="G50" s="86">
+      <c r="G50" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7933,7 +8014,7 @@
     <row r="51" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E51" s="30"/>
       <c r="F51" s="30"/>
-      <c r="G51" s="86">
+      <c r="G51" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7941,7 +8022,7 @@
     <row r="52" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E52" s="30"/>
       <c r="F52" s="30"/>
-      <c r="G52" s="86">
+      <c r="G52" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7949,7 +8030,7 @@
     <row r="53" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E53" s="30"/>
       <c r="F53" s="30"/>
-      <c r="G53" s="86">
+      <c r="G53" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7957,7 +8038,7 @@
     <row r="54" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E54" s="30"/>
       <c r="F54" s="30"/>
-      <c r="G54" s="86">
+      <c r="G54" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7965,7 +8046,7 @@
     <row r="55" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E55" s="30"/>
       <c r="F55" s="30"/>
-      <c r="G55" s="86">
+      <c r="G55" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7973,7 +8054,7 @@
     <row r="56" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E56" s="30"/>
       <c r="F56" s="30"/>
-      <c r="G56" s="86">
+      <c r="G56" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -7981,22 +8062,22 @@
     <row r="57" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E57" s="30"/>
       <c r="F57" s="30"/>
-      <c r="G57" s="86">
+      <c r="G57" s="85">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:F57">
-    <cfRule type="containsBlanks" dxfId="28" priority="3">
+    <cfRule type="containsBlanks" dxfId="32" priority="3">
       <formula>LEN(TRIM(A3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:D57">
-    <cfRule type="containsBlanks" dxfId="27" priority="1">
+    <cfRule type="containsBlanks" dxfId="31" priority="1">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="26" priority="4" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="30" priority="4" stopIfTrue="1">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8054,16 +8135,16 @@
         <v>453</v>
       </c>
       <c r="B1" s="49"/>
-      <c r="C1" s="122" t="s">
+      <c r="C1" s="121" t="s">
         <v>455</v>
       </c>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="124"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="122"/>
+      <c r="H1" s="122"/>
+      <c r="I1" s="122"/>
+      <c r="J1" s="123"/>
     </row>
     <row r="2" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="50" t="s">
@@ -8093,7 +8174,7 @@
       <c r="I2" s="50" t="s">
         <v>591</v>
       </c>
-      <c r="J2" s="81" t="s">
+      <c r="J2" s="80" t="s">
         <v>763</v>
       </c>
     </row>
@@ -9240,17 +9321,17 @@
     <mergeCell ref="C1:J1"/>
   </mergeCells>
   <conditionalFormatting sqref="A3:F3 H4:I124 E7:J121 A4:C121 D4:D208 E4:F6 F3:F6">
-    <cfRule type="containsBlanks" dxfId="25" priority="4">
+    <cfRule type="containsBlanks" dxfId="29" priority="4">
       <formula>LEN(TRIM(A3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:J124">
-    <cfRule type="containsBlanks" dxfId="24" priority="1">
+    <cfRule type="containsBlanks" dxfId="28" priority="1">
       <formula>LEN(TRIM(E3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:J6">
-    <cfRule type="containsBlanks" dxfId="23" priority="2">
+    <cfRule type="containsBlanks" dxfId="27" priority="2">
       <formula>LEN(TRIM(G3))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9618,7 +9699,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A116 C3:C116 E3:E116">
-    <cfRule type="containsBlanks" dxfId="22" priority="1">
+    <cfRule type="containsBlanks" dxfId="26" priority="1">
       <formula>LEN(TRIM(A3))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9668,13 +9749,13 @@
       <c r="A1" s="53" t="s">
         <v>453</v>
       </c>
-      <c r="B1" s="88" t="s">
+      <c r="B1" s="87" t="s">
         <v>455</v>
       </c>
       <c r="C1" s="67"/>
       <c r="D1" s="67"/>
       <c r="E1" s="67"/>
-      <c r="F1" s="80"/>
+      <c r="F1" s="79"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="50" t="s">
@@ -9683,16 +9764,16 @@
       <c r="B2" s="50" t="s">
         <v>393</v>
       </c>
-      <c r="C2" s="104" t="s">
+      <c r="C2" s="103" t="s">
         <v>906</v>
       </c>
-      <c r="D2" s="104" t="s">
+      <c r="D2" s="103" t="s">
         <v>905</v>
       </c>
-      <c r="E2" s="104" t="s">
+      <c r="E2" s="103" t="s">
         <v>694</v>
       </c>
-      <c r="F2" s="79" t="s">
+      <c r="F2" s="78" t="s">
         <v>756</v>
       </c>
     </row>
@@ -9778,17 +9859,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:F143">
-    <cfRule type="containsBlanks" dxfId="21" priority="4">
+    <cfRule type="containsBlanks" dxfId="25" priority="4">
       <formula>LEN(TRIM(A3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B143">
-    <cfRule type="containsBlanks" dxfId="20" priority="3">
+    <cfRule type="containsBlanks" dxfId="24" priority="3">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="containsBlanks" dxfId="19" priority="2">
+    <cfRule type="containsBlanks" dxfId="23" priority="2">
       <formula>LEN(TRIM(F2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9839,14 +9920,14 @@
       <c r="A1" s="53" t="s">
         <v>453</v>
       </c>
-      <c r="B1" s="125" t="s">
+      <c r="B1" s="124" t="s">
         <v>609</v>
       </c>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="125"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
     </row>
     <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="50" t="s">
@@ -9864,7 +9945,7 @@
       <c r="E2" s="54" t="s">
         <v>391</v>
       </c>
-      <c r="F2" s="83"/>
+      <c r="F2" s="82"/>
     </row>
     <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -9950,18 +10031,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="115" t="s">
         <v>475</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="117"/>
-      <c r="J1" s="118"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
+      <c r="I1" s="116"/>
+      <c r="J1" s="117"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="32" t="s">
@@ -9986,16 +10067,16 @@
         <v>476</v>
       </c>
       <c r="B3"/>
-      <c r="C3" s="119" t="s">
+      <c r="C3" s="118" t="s">
         <v>487</v>
       </c>
-      <c r="D3" s="119"/>
-      <c r="E3" s="119"/>
-      <c r="F3" s="119"/>
-      <c r="G3" s="119"/>
-      <c r="H3" s="119"/>
-      <c r="I3" s="119"/>
-      <c r="J3" s="120"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
+      <c r="I3" s="118"/>
+      <c r="J3" s="119"/>
       <c r="O3" s="31" t="s">
         <v>493</v>
       </c>
@@ -10012,507 +10093,507 @@
         <v>478</v>
       </c>
       <c r="B4"/>
-      <c r="C4" s="119" t="s">
+      <c r="C4" s="118" t="s">
         <v>488</v>
       </c>
-      <c r="D4" s="119"/>
-      <c r="E4" s="119"/>
-      <c r="F4" s="119"/>
-      <c r="G4" s="119"/>
-      <c r="H4" s="119"/>
-      <c r="I4" s="119"/>
-      <c r="J4" s="120"/>
-      <c r="O4" s="110" t="s">
+      <c r="D4" s="118"/>
+      <c r="E4" s="118"/>
+      <c r="F4" s="118"/>
+      <c r="G4" s="118"/>
+      <c r="H4" s="118"/>
+      <c r="I4" s="118"/>
+      <c r="J4" s="119"/>
+      <c r="O4" s="109" t="s">
         <v>494</v>
       </c>
-      <c r="P4" s="111"/>
-      <c r="Q4" s="111"/>
-      <c r="R4" s="111"/>
-      <c r="S4" s="111"/>
-      <c r="T4" s="111"/>
-      <c r="U4" s="111"/>
-      <c r="V4" s="112"/>
-      <c r="W4" s="87"/>
+      <c r="P4" s="110"/>
+      <c r="Q4" s="110"/>
+      <c r="R4" s="110"/>
+      <c r="S4" s="110"/>
+      <c r="T4" s="110"/>
+      <c r="U4" s="110"/>
+      <c r="V4" s="111"/>
+      <c r="W4" s="86"/>
     </row>
     <row r="5" spans="1:23" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
         <v>486</v>
       </c>
       <c r="B5"/>
-      <c r="C5" s="119" t="s">
+      <c r="C5" s="118" t="s">
         <v>489</v>
       </c>
-      <c r="D5" s="119"/>
-      <c r="E5" s="119"/>
-      <c r="F5" s="119"/>
-      <c r="G5" s="119"/>
-      <c r="H5" s="119"/>
-      <c r="I5" s="119"/>
-      <c r="J5" s="120"/>
-      <c r="O5" s="110"/>
-      <c r="P5" s="111"/>
-      <c r="Q5" s="111"/>
-      <c r="R5" s="111"/>
-      <c r="S5" s="111"/>
-      <c r="T5" s="111"/>
-      <c r="U5" s="111"/>
-      <c r="V5" s="112"/>
+      <c r="D5" s="118"/>
+      <c r="E5" s="118"/>
+      <c r="F5" s="118"/>
+      <c r="G5" s="118"/>
+      <c r="H5" s="118"/>
+      <c r="I5" s="118"/>
+      <c r="J5" s="119"/>
+      <c r="O5" s="109"/>
+      <c r="P5" s="110"/>
+      <c r="Q5" s="110"/>
+      <c r="R5" s="110"/>
+      <c r="S5" s="110"/>
+      <c r="T5" s="110"/>
+      <c r="U5" s="110"/>
+      <c r="V5" s="111"/>
     </row>
     <row r="6" spans="1:23" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="29" t="s">
         <v>477</v>
       </c>
       <c r="B6"/>
-      <c r="C6" s="119" t="s">
+      <c r="C6" s="118" t="s">
         <v>490</v>
       </c>
-      <c r="D6" s="119"/>
-      <c r="E6" s="119"/>
-      <c r="F6" s="119"/>
-      <c r="G6" s="119"/>
-      <c r="H6" s="119"/>
-      <c r="I6" s="119"/>
-      <c r="J6" s="120"/>
-      <c r="O6" s="110"/>
-      <c r="P6" s="111"/>
-      <c r="Q6" s="111"/>
-      <c r="R6" s="111"/>
-      <c r="S6" s="111"/>
-      <c r="T6" s="111"/>
-      <c r="U6" s="111"/>
-      <c r="V6" s="112"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="118"/>
+      <c r="F6" s="118"/>
+      <c r="G6" s="118"/>
+      <c r="H6" s="118"/>
+      <c r="I6" s="118"/>
+      <c r="J6" s="119"/>
+      <c r="O6" s="109"/>
+      <c r="P6" s="110"/>
+      <c r="Q6" s="110"/>
+      <c r="R6" s="110"/>
+      <c r="S6" s="110"/>
+      <c r="T6" s="110"/>
+      <c r="U6" s="110"/>
+      <c r="V6" s="111"/>
     </row>
     <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
         <v>485</v>
       </c>
       <c r="B7"/>
-      <c r="C7" s="119" t="s">
+      <c r="C7" s="118" t="s">
         <v>492</v>
       </c>
-      <c r="D7" s="119"/>
-      <c r="E7" s="119"/>
-      <c r="F7" s="119"/>
-      <c r="G7" s="119"/>
-      <c r="H7" s="119"/>
-      <c r="I7" s="119"/>
-      <c r="J7" s="120"/>
-      <c r="O7" s="110"/>
-      <c r="P7" s="111"/>
-      <c r="Q7" s="111"/>
-      <c r="R7" s="111"/>
-      <c r="S7" s="111"/>
-      <c r="T7" s="111"/>
-      <c r="U7" s="111"/>
-      <c r="V7" s="112"/>
+      <c r="D7" s="118"/>
+      <c r="E7" s="118"/>
+      <c r="F7" s="118"/>
+      <c r="G7" s="118"/>
+      <c r="H7" s="118"/>
+      <c r="I7" s="118"/>
+      <c r="J7" s="119"/>
+      <c r="O7" s="109"/>
+      <c r="P7" s="110"/>
+      <c r="Q7" s="110"/>
+      <c r="R7" s="110"/>
+      <c r="S7" s="110"/>
+      <c r="T7" s="110"/>
+      <c r="U7" s="110"/>
+      <c r="V7" s="111"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A8" s="93" t="s">
+      <c r="A8" s="92" t="s">
         <v>479</v>
       </c>
       <c r="B8"/>
-      <c r="C8" s="121" t="s">
+      <c r="C8" s="120" t="s">
         <v>817</v>
       </c>
-      <c r="D8" s="119"/>
-      <c r="E8" s="119"/>
-      <c r="F8" s="119"/>
-      <c r="G8" s="119"/>
-      <c r="H8" s="119"/>
-      <c r="I8" s="119"/>
-      <c r="J8" s="120"/>
-      <c r="O8" s="110"/>
-      <c r="P8" s="111"/>
-      <c r="Q8" s="111"/>
-      <c r="R8" s="111"/>
-      <c r="S8" s="111"/>
-      <c r="T8" s="111"/>
-      <c r="U8" s="111"/>
-      <c r="V8" s="112"/>
+      <c r="D8" s="118"/>
+      <c r="E8" s="118"/>
+      <c r="F8" s="118"/>
+      <c r="G8" s="118"/>
+      <c r="H8" s="118"/>
+      <c r="I8" s="118"/>
+      <c r="J8" s="119"/>
+      <c r="O8" s="109"/>
+      <c r="P8" s="110"/>
+      <c r="Q8" s="110"/>
+      <c r="R8" s="110"/>
+      <c r="S8" s="110"/>
+      <c r="T8" s="110"/>
+      <c r="U8" s="110"/>
+      <c r="V8" s="111"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A9" s="94" t="s">
+      <c r="A9" s="93" t="s">
         <v>491</v>
       </c>
-      <c r="B9" s="95"/>
-      <c r="C9" s="108" t="s">
+      <c r="B9" s="94"/>
+      <c r="C9" s="107" t="s">
         <v>818</v>
       </c>
-      <c r="D9" s="108"/>
-      <c r="E9" s="108"/>
-      <c r="F9" s="108"/>
-      <c r="G9" s="108"/>
-      <c r="H9" s="108"/>
-      <c r="I9" s="108"/>
-      <c r="J9" s="109"/>
-      <c r="O9" s="110"/>
-      <c r="P9" s="111"/>
-      <c r="Q9" s="111"/>
-      <c r="R9" s="111"/>
-      <c r="S9" s="111"/>
-      <c r="T9" s="111"/>
-      <c r="U9" s="111"/>
-      <c r="V9" s="112"/>
+      <c r="D9" s="107"/>
+      <c r="E9" s="107"/>
+      <c r="F9" s="107"/>
+      <c r="G9" s="107"/>
+      <c r="H9" s="107"/>
+      <c r="I9" s="107"/>
+      <c r="J9" s="108"/>
+      <c r="O9" s="109"/>
+      <c r="P9" s="110"/>
+      <c r="Q9" s="110"/>
+      <c r="R9" s="110"/>
+      <c r="S9" s="110"/>
+      <c r="T9" s="110"/>
+      <c r="U9" s="110"/>
+      <c r="V9" s="111"/>
     </row>
     <row r="10" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="O10" s="110"/>
-      <c r="P10" s="111"/>
-      <c r="Q10" s="111"/>
-      <c r="R10" s="111"/>
-      <c r="S10" s="111"/>
-      <c r="T10" s="111"/>
-      <c r="U10" s="111"/>
-      <c r="V10" s="112"/>
+      <c r="O10" s="109"/>
+      <c r="P10" s="110"/>
+      <c r="Q10" s="110"/>
+      <c r="R10" s="110"/>
+      <c r="S10" s="110"/>
+      <c r="T10" s="110"/>
+      <c r="U10" s="110"/>
+      <c r="V10" s="111"/>
     </row>
     <row r="11" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="O11" s="110"/>
-      <c r="P11" s="111"/>
-      <c r="Q11" s="111"/>
-      <c r="R11" s="111"/>
-      <c r="S11" s="111"/>
-      <c r="T11" s="111"/>
-      <c r="U11" s="111"/>
-      <c r="V11" s="112"/>
+      <c r="O11" s="109"/>
+      <c r="P11" s="110"/>
+      <c r="Q11" s="110"/>
+      <c r="R11" s="110"/>
+      <c r="S11" s="110"/>
+      <c r="T11" s="110"/>
+      <c r="U11" s="110"/>
+      <c r="V11" s="111"/>
     </row>
     <row r="12" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="O12" s="110"/>
-      <c r="P12" s="111"/>
-      <c r="Q12" s="111"/>
-      <c r="R12" s="111"/>
-      <c r="S12" s="111"/>
-      <c r="T12" s="111"/>
-      <c r="U12" s="111"/>
-      <c r="V12" s="112"/>
+      <c r="O12" s="109"/>
+      <c r="P12" s="110"/>
+      <c r="Q12" s="110"/>
+      <c r="R12" s="110"/>
+      <c r="S12" s="110"/>
+      <c r="T12" s="110"/>
+      <c r="U12" s="110"/>
+      <c r="V12" s="111"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="O13" s="110"/>
-      <c r="P13" s="111"/>
-      <c r="Q13" s="111"/>
-      <c r="R13" s="111"/>
-      <c r="S13" s="111"/>
-      <c r="T13" s="111"/>
-      <c r="U13" s="111"/>
-      <c r="V13" s="112"/>
+      <c r="O13" s="109"/>
+      <c r="P13" s="110"/>
+      <c r="Q13" s="110"/>
+      <c r="R13" s="110"/>
+      <c r="S13" s="110"/>
+      <c r="T13" s="110"/>
+      <c r="U13" s="110"/>
+      <c r="V13" s="111"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="O14" s="110"/>
-      <c r="P14" s="111"/>
-      <c r="Q14" s="111"/>
-      <c r="R14" s="111"/>
-      <c r="S14" s="111"/>
-      <c r="T14" s="111"/>
-      <c r="U14" s="111"/>
-      <c r="V14" s="112"/>
+      <c r="O14" s="109"/>
+      <c r="P14" s="110"/>
+      <c r="Q14" s="110"/>
+      <c r="R14" s="110"/>
+      <c r="S14" s="110"/>
+      <c r="T14" s="110"/>
+      <c r="U14" s="110"/>
+      <c r="V14" s="111"/>
     </row>
     <row r="15" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="O15" s="110"/>
-      <c r="P15" s="111"/>
-      <c r="Q15" s="111"/>
-      <c r="R15" s="111"/>
-      <c r="S15" s="111"/>
-      <c r="T15" s="111"/>
-      <c r="U15" s="111"/>
-      <c r="V15" s="112"/>
+      <c r="O15" s="109"/>
+      <c r="P15" s="110"/>
+      <c r="Q15" s="110"/>
+      <c r="R15" s="110"/>
+      <c r="S15" s="110"/>
+      <c r="T15" s="110"/>
+      <c r="U15" s="110"/>
+      <c r="V15" s="111"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="O16" s="110"/>
-      <c r="P16" s="111"/>
-      <c r="Q16" s="111"/>
-      <c r="R16" s="111"/>
-      <c r="S16" s="111"/>
-      <c r="T16" s="111"/>
-      <c r="U16" s="111"/>
-      <c r="V16" s="112"/>
+      <c r="O16" s="109"/>
+      <c r="P16" s="110"/>
+      <c r="Q16" s="110"/>
+      <c r="R16" s="110"/>
+      <c r="S16" s="110"/>
+      <c r="T16" s="110"/>
+      <c r="U16" s="110"/>
+      <c r="V16" s="111"/>
     </row>
     <row r="17" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O17" s="110"/>
-      <c r="P17" s="111"/>
-      <c r="Q17" s="111"/>
-      <c r="R17" s="111"/>
-      <c r="S17" s="111"/>
-      <c r="T17" s="111"/>
-      <c r="U17" s="111"/>
-      <c r="V17" s="112"/>
+      <c r="O17" s="109"/>
+      <c r="P17" s="110"/>
+      <c r="Q17" s="110"/>
+      <c r="R17" s="110"/>
+      <c r="S17" s="110"/>
+      <c r="T17" s="110"/>
+      <c r="U17" s="110"/>
+      <c r="V17" s="111"/>
     </row>
     <row r="18" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O18" s="110"/>
-      <c r="P18" s="111"/>
-      <c r="Q18" s="111"/>
-      <c r="R18" s="111"/>
-      <c r="S18" s="111"/>
-      <c r="T18" s="111"/>
-      <c r="U18" s="111"/>
-      <c r="V18" s="112"/>
+      <c r="O18" s="109"/>
+      <c r="P18" s="110"/>
+      <c r="Q18" s="110"/>
+      <c r="R18" s="110"/>
+      <c r="S18" s="110"/>
+      <c r="T18" s="110"/>
+      <c r="U18" s="110"/>
+      <c r="V18" s="111"/>
     </row>
     <row r="19" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O19" s="110"/>
-      <c r="P19" s="111"/>
-      <c r="Q19" s="111"/>
-      <c r="R19" s="111"/>
-      <c r="S19" s="111"/>
-      <c r="T19" s="111"/>
-      <c r="U19" s="111"/>
-      <c r="V19" s="112"/>
+      <c r="O19" s="109"/>
+      <c r="P19" s="110"/>
+      <c r="Q19" s="110"/>
+      <c r="R19" s="110"/>
+      <c r="S19" s="110"/>
+      <c r="T19" s="110"/>
+      <c r="U19" s="110"/>
+      <c r="V19" s="111"/>
     </row>
     <row r="20" spans="15:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="O20" s="110"/>
-      <c r="P20" s="111"/>
-      <c r="Q20" s="111"/>
-      <c r="R20" s="111"/>
-      <c r="S20" s="111"/>
-      <c r="T20" s="111"/>
-      <c r="U20" s="111"/>
-      <c r="V20" s="112"/>
+      <c r="O20" s="109"/>
+      <c r="P20" s="110"/>
+      <c r="Q20" s="110"/>
+      <c r="R20" s="110"/>
+      <c r="S20" s="110"/>
+      <c r="T20" s="110"/>
+      <c r="U20" s="110"/>
+      <c r="V20" s="111"/>
     </row>
     <row r="21" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O21" s="110"/>
-      <c r="P21" s="111"/>
-      <c r="Q21" s="111"/>
-      <c r="R21" s="111"/>
-      <c r="S21" s="111"/>
-      <c r="T21" s="111"/>
-      <c r="U21" s="111"/>
-      <c r="V21" s="112"/>
+      <c r="O21" s="109"/>
+      <c r="P21" s="110"/>
+      <c r="Q21" s="110"/>
+      <c r="R21" s="110"/>
+      <c r="S21" s="110"/>
+      <c r="T21" s="110"/>
+      <c r="U21" s="110"/>
+      <c r="V21" s="111"/>
     </row>
     <row r="22" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O22" s="110"/>
-      <c r="P22" s="111"/>
-      <c r="Q22" s="111"/>
-      <c r="R22" s="111"/>
-      <c r="S22" s="111"/>
-      <c r="T22" s="111"/>
-      <c r="U22" s="111"/>
-      <c r="V22" s="112"/>
+      <c r="O22" s="109"/>
+      <c r="P22" s="110"/>
+      <c r="Q22" s="110"/>
+      <c r="R22" s="110"/>
+      <c r="S22" s="110"/>
+      <c r="T22" s="110"/>
+      <c r="U22" s="110"/>
+      <c r="V22" s="111"/>
     </row>
     <row r="23" spans="15:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="O23" s="110"/>
-      <c r="P23" s="111"/>
-      <c r="Q23" s="111"/>
-      <c r="R23" s="111"/>
-      <c r="S23" s="111"/>
-      <c r="T23" s="111"/>
-      <c r="U23" s="111"/>
-      <c r="V23" s="112"/>
+      <c r="O23" s="109"/>
+      <c r="P23" s="110"/>
+      <c r="Q23" s="110"/>
+      <c r="R23" s="110"/>
+      <c r="S23" s="110"/>
+      <c r="T23" s="110"/>
+      <c r="U23" s="110"/>
+      <c r="V23" s="111"/>
     </row>
     <row r="24" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O24" s="110"/>
-      <c r="P24" s="111"/>
-      <c r="Q24" s="111"/>
-      <c r="R24" s="111"/>
-      <c r="S24" s="111"/>
-      <c r="T24" s="111"/>
-      <c r="U24" s="111"/>
-      <c r="V24" s="112"/>
+      <c r="O24" s="109"/>
+      <c r="P24" s="110"/>
+      <c r="Q24" s="110"/>
+      <c r="R24" s="110"/>
+      <c r="S24" s="110"/>
+      <c r="T24" s="110"/>
+      <c r="U24" s="110"/>
+      <c r="V24" s="111"/>
     </row>
     <row r="25" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O25" s="110"/>
-      <c r="P25" s="111"/>
-      <c r="Q25" s="111"/>
-      <c r="R25" s="111"/>
-      <c r="S25" s="111"/>
-      <c r="T25" s="111"/>
-      <c r="U25" s="111"/>
-      <c r="V25" s="112"/>
+      <c r="O25" s="109"/>
+      <c r="P25" s="110"/>
+      <c r="Q25" s="110"/>
+      <c r="R25" s="110"/>
+      <c r="S25" s="110"/>
+      <c r="T25" s="110"/>
+      <c r="U25" s="110"/>
+      <c r="V25" s="111"/>
     </row>
     <row r="26" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O26" s="110"/>
-      <c r="P26" s="111"/>
-      <c r="Q26" s="111"/>
-      <c r="R26" s="111"/>
-      <c r="S26" s="111"/>
-      <c r="T26" s="111"/>
-      <c r="U26" s="111"/>
-      <c r="V26" s="112"/>
+      <c r="O26" s="109"/>
+      <c r="P26" s="110"/>
+      <c r="Q26" s="110"/>
+      <c r="R26" s="110"/>
+      <c r="S26" s="110"/>
+      <c r="T26" s="110"/>
+      <c r="U26" s="110"/>
+      <c r="V26" s="111"/>
     </row>
     <row r="27" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O27" s="110"/>
-      <c r="P27" s="111"/>
-      <c r="Q27" s="111"/>
-      <c r="R27" s="111"/>
-      <c r="S27" s="111"/>
-      <c r="T27" s="111"/>
-      <c r="U27" s="111"/>
-      <c r="V27" s="112"/>
+      <c r="O27" s="109"/>
+      <c r="P27" s="110"/>
+      <c r="Q27" s="110"/>
+      <c r="R27" s="110"/>
+      <c r="S27" s="110"/>
+      <c r="T27" s="110"/>
+      <c r="U27" s="110"/>
+      <c r="V27" s="111"/>
     </row>
     <row r="28" spans="15:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="O28" s="110"/>
-      <c r="P28" s="111"/>
-      <c r="Q28" s="111"/>
-      <c r="R28" s="111"/>
-      <c r="S28" s="111"/>
-      <c r="T28" s="111"/>
-      <c r="U28" s="111"/>
-      <c r="V28" s="112"/>
+      <c r="O28" s="109"/>
+      <c r="P28" s="110"/>
+      <c r="Q28" s="110"/>
+      <c r="R28" s="110"/>
+      <c r="S28" s="110"/>
+      <c r="T28" s="110"/>
+      <c r="U28" s="110"/>
+      <c r="V28" s="111"/>
     </row>
     <row r="29" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O29" s="110"/>
-      <c r="P29" s="111"/>
-      <c r="Q29" s="111"/>
-      <c r="R29" s="111"/>
-      <c r="S29" s="111"/>
-      <c r="T29" s="111"/>
-      <c r="U29" s="111"/>
-      <c r="V29" s="112"/>
+      <c r="O29" s="109"/>
+      <c r="P29" s="110"/>
+      <c r="Q29" s="110"/>
+      <c r="R29" s="110"/>
+      <c r="S29" s="110"/>
+      <c r="T29" s="110"/>
+      <c r="U29" s="110"/>
+      <c r="V29" s="111"/>
     </row>
     <row r="30" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O30" s="110"/>
-      <c r="P30" s="111"/>
-      <c r="Q30" s="111"/>
-      <c r="R30" s="111"/>
-      <c r="S30" s="111"/>
-      <c r="T30" s="111"/>
-      <c r="U30" s="111"/>
-      <c r="V30" s="112"/>
+      <c r="O30" s="109"/>
+      <c r="P30" s="110"/>
+      <c r="Q30" s="110"/>
+      <c r="R30" s="110"/>
+      <c r="S30" s="110"/>
+      <c r="T30" s="110"/>
+      <c r="U30" s="110"/>
+      <c r="V30" s="111"/>
     </row>
     <row r="31" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O31" s="110"/>
-      <c r="P31" s="111"/>
-      <c r="Q31" s="111"/>
-      <c r="R31" s="111"/>
-      <c r="S31" s="111"/>
-      <c r="T31" s="111"/>
-      <c r="U31" s="111"/>
-      <c r="V31" s="112"/>
+      <c r="O31" s="109"/>
+      <c r="P31" s="110"/>
+      <c r="Q31" s="110"/>
+      <c r="R31" s="110"/>
+      <c r="S31" s="110"/>
+      <c r="T31" s="110"/>
+      <c r="U31" s="110"/>
+      <c r="V31" s="111"/>
     </row>
     <row r="32" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O32" s="110"/>
-      <c r="P32" s="111"/>
-      <c r="Q32" s="111"/>
-      <c r="R32" s="111"/>
-      <c r="S32" s="111"/>
-      <c r="T32" s="111"/>
-      <c r="U32" s="111"/>
-      <c r="V32" s="112"/>
+      <c r="O32" s="109"/>
+      <c r="P32" s="110"/>
+      <c r="Q32" s="110"/>
+      <c r="R32" s="110"/>
+      <c r="S32" s="110"/>
+      <c r="T32" s="110"/>
+      <c r="U32" s="110"/>
+      <c r="V32" s="111"/>
     </row>
     <row r="33" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O33" s="110"/>
-      <c r="P33" s="111"/>
-      <c r="Q33" s="111"/>
-      <c r="R33" s="111"/>
-      <c r="S33" s="111"/>
-      <c r="T33" s="111"/>
-      <c r="U33" s="111"/>
-      <c r="V33" s="112"/>
+      <c r="O33" s="109"/>
+      <c r="P33" s="110"/>
+      <c r="Q33" s="110"/>
+      <c r="R33" s="110"/>
+      <c r="S33" s="110"/>
+      <c r="T33" s="110"/>
+      <c r="U33" s="110"/>
+      <c r="V33" s="111"/>
     </row>
     <row r="34" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O34" s="110"/>
-      <c r="P34" s="111"/>
-      <c r="Q34" s="111"/>
-      <c r="R34" s="111"/>
-      <c r="S34" s="111"/>
-      <c r="T34" s="111"/>
-      <c r="U34" s="111"/>
-      <c r="V34" s="112"/>
+      <c r="O34" s="109"/>
+      <c r="P34" s="110"/>
+      <c r="Q34" s="110"/>
+      <c r="R34" s="110"/>
+      <c r="S34" s="110"/>
+      <c r="T34" s="110"/>
+      <c r="U34" s="110"/>
+      <c r="V34" s="111"/>
     </row>
     <row r="35" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O35" s="110"/>
-      <c r="P35" s="111"/>
-      <c r="Q35" s="111"/>
-      <c r="R35" s="111"/>
-      <c r="S35" s="111"/>
-      <c r="T35" s="111"/>
-      <c r="U35" s="111"/>
-      <c r="V35" s="112"/>
+      <c r="O35" s="109"/>
+      <c r="P35" s="110"/>
+      <c r="Q35" s="110"/>
+      <c r="R35" s="110"/>
+      <c r="S35" s="110"/>
+      <c r="T35" s="110"/>
+      <c r="U35" s="110"/>
+      <c r="V35" s="111"/>
     </row>
     <row r="36" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O36" s="110"/>
-      <c r="P36" s="111"/>
-      <c r="Q36" s="111"/>
-      <c r="R36" s="111"/>
-      <c r="S36" s="111"/>
-      <c r="T36" s="111"/>
-      <c r="U36" s="111"/>
-      <c r="V36" s="112"/>
+      <c r="O36" s="109"/>
+      <c r="P36" s="110"/>
+      <c r="Q36" s="110"/>
+      <c r="R36" s="110"/>
+      <c r="S36" s="110"/>
+      <c r="T36" s="110"/>
+      <c r="U36" s="110"/>
+      <c r="V36" s="111"/>
     </row>
     <row r="37" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O37" s="110"/>
-      <c r="P37" s="111"/>
-      <c r="Q37" s="111"/>
-      <c r="R37" s="111"/>
-      <c r="S37" s="111"/>
-      <c r="T37" s="111"/>
-      <c r="U37" s="111"/>
-      <c r="V37" s="112"/>
+      <c r="O37" s="109"/>
+      <c r="P37" s="110"/>
+      <c r="Q37" s="110"/>
+      <c r="R37" s="110"/>
+      <c r="S37" s="110"/>
+      <c r="T37" s="110"/>
+      <c r="U37" s="110"/>
+      <c r="V37" s="111"/>
     </row>
     <row r="38" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O38" s="110"/>
-      <c r="P38" s="111"/>
-      <c r="Q38" s="111"/>
-      <c r="R38" s="111"/>
-      <c r="S38" s="111"/>
-      <c r="T38" s="111"/>
-      <c r="U38" s="111"/>
-      <c r="V38" s="112"/>
+      <c r="O38" s="109"/>
+      <c r="P38" s="110"/>
+      <c r="Q38" s="110"/>
+      <c r="R38" s="110"/>
+      <c r="S38" s="110"/>
+      <c r="T38" s="110"/>
+      <c r="U38" s="110"/>
+      <c r="V38" s="111"/>
     </row>
     <row r="39" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O39" s="110"/>
-      <c r="P39" s="111"/>
-      <c r="Q39" s="111"/>
-      <c r="R39" s="111"/>
-      <c r="S39" s="111"/>
-      <c r="T39" s="111"/>
-      <c r="U39" s="111"/>
-      <c r="V39" s="112"/>
+      <c r="O39" s="109"/>
+      <c r="P39" s="110"/>
+      <c r="Q39" s="110"/>
+      <c r="R39" s="110"/>
+      <c r="S39" s="110"/>
+      <c r="T39" s="110"/>
+      <c r="U39" s="110"/>
+      <c r="V39" s="111"/>
     </row>
     <row r="40" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O40" s="110"/>
-      <c r="P40" s="111"/>
-      <c r="Q40" s="111"/>
-      <c r="R40" s="111"/>
-      <c r="S40" s="111"/>
-      <c r="T40" s="111"/>
-      <c r="U40" s="111"/>
-      <c r="V40" s="112"/>
+      <c r="O40" s="109"/>
+      <c r="P40" s="110"/>
+      <c r="Q40" s="110"/>
+      <c r="R40" s="110"/>
+      <c r="S40" s="110"/>
+      <c r="T40" s="110"/>
+      <c r="U40" s="110"/>
+      <c r="V40" s="111"/>
     </row>
     <row r="41" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O41" s="110"/>
-      <c r="P41" s="111"/>
-      <c r="Q41" s="111"/>
-      <c r="R41" s="111"/>
-      <c r="S41" s="111"/>
-      <c r="T41" s="111"/>
-      <c r="U41" s="111"/>
-      <c r="V41" s="112"/>
+      <c r="O41" s="109"/>
+      <c r="P41" s="110"/>
+      <c r="Q41" s="110"/>
+      <c r="R41" s="110"/>
+      <c r="S41" s="110"/>
+      <c r="T41" s="110"/>
+      <c r="U41" s="110"/>
+      <c r="V41" s="111"/>
     </row>
     <row r="42" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O42" s="110"/>
-      <c r="P42" s="111"/>
-      <c r="Q42" s="111"/>
-      <c r="R42" s="111"/>
-      <c r="S42" s="111"/>
-      <c r="T42" s="111"/>
-      <c r="U42" s="111"/>
-      <c r="V42" s="112"/>
+      <c r="O42" s="109"/>
+      <c r="P42" s="110"/>
+      <c r="Q42" s="110"/>
+      <c r="R42" s="110"/>
+      <c r="S42" s="110"/>
+      <c r="T42" s="110"/>
+      <c r="U42" s="110"/>
+      <c r="V42" s="111"/>
     </row>
     <row r="43" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O43" s="110"/>
-      <c r="P43" s="111"/>
-      <c r="Q43" s="111"/>
-      <c r="R43" s="111"/>
-      <c r="S43" s="111"/>
-      <c r="T43" s="111"/>
-      <c r="U43" s="111"/>
-      <c r="V43" s="112"/>
+      <c r="O43" s="109"/>
+      <c r="P43" s="110"/>
+      <c r="Q43" s="110"/>
+      <c r="R43" s="110"/>
+      <c r="S43" s="110"/>
+      <c r="T43" s="110"/>
+      <c r="U43" s="110"/>
+      <c r="V43" s="111"/>
     </row>
     <row r="44" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O44" s="110"/>
-      <c r="P44" s="111"/>
-      <c r="Q44" s="111"/>
-      <c r="R44" s="111"/>
-      <c r="S44" s="111"/>
-      <c r="T44" s="111"/>
-      <c r="U44" s="111"/>
-      <c r="V44" s="112"/>
+      <c r="O44" s="109"/>
+      <c r="P44" s="110"/>
+      <c r="Q44" s="110"/>
+      <c r="R44" s="110"/>
+      <c r="S44" s="110"/>
+      <c r="T44" s="110"/>
+      <c r="U44" s="110"/>
+      <c r="V44" s="111"/>
     </row>
     <row r="45" spans="15:22" x14ac:dyDescent="0.2">
-      <c r="O45" s="113"/>
-      <c r="P45" s="114"/>
-      <c r="Q45" s="114"/>
-      <c r="R45" s="114"/>
-      <c r="S45" s="114"/>
-      <c r="T45" s="114"/>
-      <c r="U45" s="114"/>
-      <c r="V45" s="115"/>
+      <c r="O45" s="112"/>
+      <c r="P45" s="113"/>
+      <c r="Q45" s="113"/>
+      <c r="R45" s="113"/>
+      <c r="S45" s="113"/>
+      <c r="T45" s="113"/>
+      <c r="U45" s="113"/>
+      <c r="V45" s="114"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -10527,7 +10608,7 @@
     <mergeCell ref="C8:J8"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:B9">
-    <cfRule type="containsBlanks" dxfId="53" priority="1">
+    <cfRule type="containsBlanks" dxfId="57" priority="1">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10583,16 +10664,16 @@
       <c r="A1" s="47" t="s">
         <v>547</v>
       </c>
-      <c r="B1" s="123" t="s">
+      <c r="B1" s="122" t="s">
         <v>506</v>
       </c>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="122"/>
+      <c r="H1" s="122"/>
+      <c r="I1" s="122"/>
       <c r="J1" s="56"/>
       <c r="K1" s="56"/>
       <c r="L1" s="56"/>
@@ -11792,8 +11873,8 @@
   </sheetPr>
   <dimension ref="A1:P366"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A330" workbookViewId="0">
-      <selection activeCell="G341" sqref="G341"/>
+    <sheetView topLeftCell="A330" workbookViewId="0">
+      <selection activeCell="C348" sqref="C348"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11808,72 +11889,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="128" t="s">
+      <c r="A1" s="127" t="s">
         <v>692</v>
       </c>
-      <c r="B1" s="128"/>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
-      <c r="E1" s="128"/>
-      <c r="F1" s="128"/>
-      <c r="G1" s="128"/>
-      <c r="H1" s="128"/>
-      <c r="I1" s="128"/>
-      <c r="J1" s="128"/>
-      <c r="K1" s="128"/>
-      <c r="L1" s="128"/>
-      <c r="M1" s="128"/>
-      <c r="N1" s="128"/>
-      <c r="O1" s="128"/>
-      <c r="P1" s="128"/>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="127"/>
+      <c r="H1" s="127"/>
+      <c r="I1" s="127"/>
+      <c r="J1" s="127"/>
+      <c r="K1" s="127"/>
+      <c r="L1" s="127"/>
+      <c r="M1" s="127"/>
+      <c r="N1" s="127"/>
+      <c r="O1" s="127"/>
+      <c r="P1" s="127"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="78" t="s">
         <v>642</v>
       </c>
-      <c r="C2" s="79" t="s">
+      <c r="C2" s="78" t="s">
         <v>356</v>
       </c>
-      <c r="D2" s="79" t="s">
+      <c r="D2" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="104" t="s">
+      <c r="E2" s="103" t="s">
         <v>908</v>
       </c>
-      <c r="F2" s="104" t="s">
+      <c r="F2" s="103" t="s">
         <v>907</v>
       </c>
-      <c r="G2" s="104" t="s">
+      <c r="G2" s="103" t="s">
         <v>909</v>
       </c>
-      <c r="H2" s="104" t="s">
+      <c r="H2" s="103" t="s">
         <v>917</v>
       </c>
-      <c r="I2" s="79" t="s">
+      <c r="I2" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="104" t="s">
+      <c r="J2" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="79" t="s">
+      <c r="K2" s="78" t="s">
         <v>678</v>
       </c>
-      <c r="L2" s="79" t="s">
+      <c r="L2" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="79" t="s">
+      <c r="M2" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="79" t="s">
+      <c r="N2" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="79" t="s">
+      <c r="O2" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="79" t="s">
+      <c r="P2" s="78" t="s">
         <v>7</v>
       </c>
     </row>
@@ -28950,7 +29031,7 @@
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28960,9 +29041,9 @@
     <col min="3" max="3" width="46.83203125" customWidth="1"/>
     <col min="4" max="4" width="48.1640625" customWidth="1"/>
     <col min="5" max="5" width="30" customWidth="1"/>
-    <col min="6" max="6" width="24.33203125" style="83" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" style="82" customWidth="1"/>
     <col min="7" max="16" width="11.5" style="5"/>
-    <col min="17" max="17" width="11.5" style="86"/>
+    <col min="17" max="17" width="11.5" style="85"/>
     <col min="18" max="18" width="21" customWidth="1"/>
     <col min="22" max="22" width="11.5" style="30"/>
     <col min="23" max="23" width="11.5" style="5"/>
@@ -28981,22 +29062,22 @@
       <c r="C1" s="47" t="s">
         <v>547</v>
       </c>
-      <c r="D1" s="84" t="s">
+      <c r="D1" s="83" t="s">
         <v>610</v>
       </c>
-      <c r="E1" s="84" t="s">
+      <c r="E1" s="83" t="s">
         <v>611</v>
       </c>
-      <c r="F1" s="123" t="s">
+      <c r="F1" s="122" t="s">
         <v>506</v>
       </c>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
-      <c r="K1" s="123"/>
-      <c r="L1" s="123"/>
-      <c r="M1" s="123"/>
+      <c r="G1" s="122"/>
+      <c r="H1" s="122"/>
+      <c r="I1" s="122"/>
+      <c r="J1" s="122"/>
+      <c r="K1" s="122"/>
+      <c r="L1" s="122"/>
+      <c r="M1" s="122"/>
       <c r="R1" s="49" t="s">
         <v>498</v>
       </c>
@@ -29026,7 +29107,7 @@
       <c r="E2" s="65" t="s">
         <v>632</v>
       </c>
-      <c r="F2" s="85" t="s">
+      <c r="F2" s="84" t="s">
         <v>919</v>
       </c>
       <c r="G2" s="59" t="s">
@@ -34362,37 +34443,37 @@
     <mergeCell ref="F1:M1"/>
   </mergeCells>
   <conditionalFormatting sqref="A15:B94">
-    <cfRule type="containsBlanks" dxfId="18" priority="9">
+    <cfRule type="containsBlanks" dxfId="22" priority="9">
       <formula>LEN(TRIM(A15))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B94">
-    <cfRule type="containsBlanks" dxfId="17" priority="5">
+    <cfRule type="containsBlanks" dxfId="21" priority="5">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21 H21 J21:J85 H23:H85 F23:F85">
-    <cfRule type="containsBlanks" dxfId="16" priority="4">
+    <cfRule type="containsBlanks" dxfId="20" priority="4">
       <formula>LEN(TRIM(F21))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L20:L85">
-    <cfRule type="containsBlanks" dxfId="15" priority="3">
+    <cfRule type="containsBlanks" dxfId="19" priority="3">
       <formula>LEN(TRIM(L20))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N20:N85">
-    <cfRule type="containsBlanks" dxfId="14" priority="2">
+    <cfRule type="containsBlanks" dxfId="18" priority="2">
       <formula>LEN(TRIM(N20))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P20:P85">
-    <cfRule type="containsBlanks" dxfId="13" priority="1">
+    <cfRule type="containsBlanks" dxfId="17" priority="1">
       <formula>LEN(TRIM(P20))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R16:R94">
-    <cfRule type="containsBlanks" dxfId="12" priority="6">
+    <cfRule type="containsBlanks" dxfId="16" priority="6">
       <formula>LEN(TRIM(R16))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -34425,11 +34506,11 @@
   </sheetPr>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView zoomScale="111" zoomScaleNormal="111" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
       <pane xSplit="12" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -34438,7 +34519,7 @@
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="12.5" customWidth="1"/>
     <col min="4" max="6" width="19.1640625" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" customWidth="1"/>
     <col min="8" max="8" width="46.5" customWidth="1"/>
     <col min="9" max="9" width="25.83203125" customWidth="1"/>
     <col min="10" max="10" width="17.6640625" customWidth="1"/>
@@ -34463,15 +34544,15 @@
       </c>
       <c r="E1" s="70"/>
       <c r="F1" s="70"/>
-      <c r="G1" s="126" t="s">
+      <c r="G1" s="125" t="s">
         <v>509</v>
       </c>
-      <c r="H1" s="126"/>
-      <c r="I1" s="126"/>
-      <c r="J1" s="126"/>
-      <c r="K1" s="126"/>
-      <c r="L1" s="126"/>
-      <c r="M1" s="126"/>
+      <c r="H1" s="125"/>
+      <c r="I1" s="125"/>
+      <c r="J1" s="125"/>
+      <c r="K1" s="125"/>
+      <c r="L1" s="125"/>
+      <c r="M1" s="125"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="43" t="s">
@@ -34514,7 +34595,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
         <v>510</v>
       </c>
@@ -34531,23 +34612,23 @@
       <c r="H3" s="7" t="s">
         <v>340</v>
       </c>
-      <c r="I3" s="7" t="s">
-        <v>342</v>
+      <c r="I3" t="s">
+        <v>911</v>
       </c>
       <c r="J3" s="7" t="s">
         <v>349</v>
       </c>
-      <c r="K3" s="7" t="s">
-        <v>349</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>352</v>
-      </c>
-      <c r="M3" s="71" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="K3" t="s">
+        <v>912</v>
+      </c>
+      <c r="L3" t="s">
+        <v>913</v>
+      </c>
+      <c r="M3" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>564</v>
       </c>
@@ -34572,20 +34653,20 @@
       <c r="H4" s="7" t="s">
         <v>340</v>
       </c>
-      <c r="I4" s="7" t="s">
-        <v>342</v>
+      <c r="I4" t="s">
+        <v>911</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>349</v>
       </c>
-      <c r="K4" s="7" t="s">
-        <v>349</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>352</v>
-      </c>
-      <c r="M4" s="71" t="s">
-        <v>511</v>
+      <c r="K4" t="s">
+        <v>912</v>
+      </c>
+      <c r="L4" t="s">
+        <v>913</v>
+      </c>
+      <c r="M4" t="s">
+        <v>913</v>
       </c>
     </row>
   </sheetData>
@@ -34593,8 +34674,28 @@
     <mergeCell ref="G1:M1"/>
   </mergeCells>
   <conditionalFormatting sqref="A5:M91 A4:E4">
-    <cfRule type="containsBlanks" dxfId="11" priority="1">
+    <cfRule type="containsBlanks" dxfId="15" priority="5">
       <formula>LEN(TRIM(A4))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I4">
+    <cfRule type="containsBlanks" dxfId="3" priority="4">
+      <formula>LEN(TRIM(I3))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3:K4">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(K3))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L3:L4">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(L3))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M4">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(M3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -34607,7 +34708,7 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="14">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="11">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1A0808F8-2DDD-486B-BCCA-A4E8E8C230D2}">
           <x14:formula1>
             <xm:f>Constructions!$A:$A</xm:f>
@@ -34662,29 +34763,11 @@
           </x14:formula1>
           <xm:sqref>G3:G4 F4</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{848EC710-F0F1-544C-9EC8-0FC96FDFFD3C}">
-          <x14:formula1>
-            <xm:f>Constructions!$C$2:$C$11</xm:f>
-          </x14:formula1>
-          <xm:sqref>I3:I4</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4E2E5BCE-B11C-4946-A7C0-2FEA6E6D73C7}">
           <x14:formula1>
             <xm:f>Constructions!$D$2:$D$11</xm:f>
           </x14:formula1>
-          <xm:sqref>J3:K4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{478A521D-93DD-B844-9A66-C5D19B3455C0}">
-          <x14:formula1>
-            <xm:f>Constructions!$E$2:$E$9</xm:f>
-          </x14:formula1>
-          <xm:sqref>L3:L4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8F7BF4EB-8A6F-104D-899C-81101273BF41}">
-          <x14:formula1>
-            <xm:f>Constructions!$F$2:$F$10</xm:f>
-          </x14:formula1>
-          <xm:sqref>M3:M4</xm:sqref>
+          <xm:sqref>J3:J4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D750347B-97E6-498F-B9F4-0F21FAE21836}">
           <x14:formula1>
@@ -34731,13 +34814,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="79" t="s">
         <v>821</v>
       </c>
-      <c r="B1" s="80" t="s">
+      <c r="B1" s="79" t="s">
         <v>822</v>
       </c>
-      <c r="C1" s="80" t="s">
+      <c r="C1" s="79" t="s">
         <v>823</v>
       </c>
     </row>
@@ -34748,68 +34831,68 @@
       <c r="B2" s="50" t="s">
         <v>819</v>
       </c>
-      <c r="C2" s="90" t="s">
+      <c r="C2" s="89" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="96" t="s">
+      <c r="A3" s="95" t="s">
         <v>824</v>
       </c>
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="95" t="s">
         <v>792</v>
       </c>
-      <c r="C3" s="97">
+      <c r="C3" s="96">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="96" t="s">
+      <c r="A4" s="95" t="s">
         <v>824</v>
       </c>
-      <c r="B4" s="96" t="s">
+      <c r="B4" s="95" t="s">
         <v>795</v>
       </c>
-      <c r="C4" s="97">
+      <c r="C4" s="96">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="96" t="s">
+      <c r="A5" s="95" t="s">
         <v>824</v>
       </c>
-      <c r="B5" s="96" t="s">
+      <c r="B5" s="95" t="s">
         <v>798</v>
       </c>
-      <c r="C5" s="97">
+      <c r="C5" s="96">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="96" t="s">
+      <c r="A6" s="95" t="s">
         <v>824</v>
       </c>
-      <c r="B6" s="96" t="s">
+      <c r="B6" s="95" t="s">
         <v>796</v>
       </c>
-      <c r="C6" s="97">
+      <c r="C6" s="96">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="96" t="s">
+      <c r="A7" s="95" t="s">
         <v>824</v>
       </c>
-      <c r="B7" s="96" t="s">
+      <c r="B7" s="95" t="s">
         <v>797</v>
       </c>
-      <c r="C7" s="97">
+      <c r="C7" s="96">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B4">
-    <cfRule type="containsBlanks" dxfId="10" priority="1">
+    <cfRule type="containsBlanks" dxfId="14" priority="1">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -34836,39 +34919,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="71" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="79" t="s">
         <v>750</v>
       </c>
-      <c r="B1" s="80" t="s">
+      <c r="B1" s="79" t="s">
         <v>751</v>
       </c>
-      <c r="C1" s="122" t="s">
+      <c r="C1" s="121" t="s">
         <v>752</v>
       </c>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="123"/>
-      <c r="I1" s="123"/>
-      <c r="J1" s="123"/>
-      <c r="K1" s="123"/>
-      <c r="L1" s="123"/>
-      <c r="M1" s="123"/>
-      <c r="N1" s="123"/>
-      <c r="O1" s="123"/>
-      <c r="P1" s="123"/>
-      <c r="Q1" s="123"/>
-      <c r="R1" s="123"/>
-      <c r="S1" s="123"/>
-      <c r="T1" s="123"/>
-      <c r="U1" s="123"/>
-      <c r="V1" s="123"/>
-      <c r="W1" s="123"/>
-      <c r="X1" s="123"/>
-      <c r="Y1" s="123"/>
-      <c r="Z1" s="123"/>
-      <c r="AA1" s="124"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="122"/>
+      <c r="H1" s="122"/>
+      <c r="I1" s="122"/>
+      <c r="J1" s="122"/>
+      <c r="K1" s="122"/>
+      <c r="L1" s="122"/>
+      <c r="M1" s="122"/>
+      <c r="N1" s="122"/>
+      <c r="O1" s="122"/>
+      <c r="P1" s="122"/>
+      <c r="Q1" s="122"/>
+      <c r="R1" s="122"/>
+      <c r="S1" s="122"/>
+      <c r="T1" s="122"/>
+      <c r="U1" s="122"/>
+      <c r="V1" s="122"/>
+      <c r="W1" s="122"/>
+      <c r="X1" s="122"/>
+      <c r="Y1" s="122"/>
+      <c r="Z1" s="122"/>
+      <c r="AA1" s="123"/>
     </row>
     <row r="2" spans="1:27" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="50" t="s">
@@ -35045,103 +35128,103 @@
       </c>
       <c r="C4">
         <f ca="1">RANDBETWEEN(0,100)/100</f>
-        <v>0.94</v>
+        <v>0.2</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:AA4" ca="1" si="0">RANDBETWEEN(0,100)/100</f>
-        <v>0.23</v>
+        <v>0.84</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.04</v>
+        <v>0.99</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.9</v>
+        <v>0.08</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.27</v>
+        <v>0.21</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>0.87</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1</v>
+        <v>0.22</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.79</v>
+        <v>0.16</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.86</v>
+        <v>0.69</v>
       </c>
       <c r="L4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.44</v>
+        <v>0.09</v>
       </c>
       <c r="M4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.45</v>
+        <v>0.37</v>
       </c>
       <c r="N4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.81</v>
+        <v>0.31</v>
       </c>
       <c r="O4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.72</v>
+        <v>0.82</v>
       </c>
       <c r="P4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.4</v>
+        <v>0.86</v>
       </c>
       <c r="Q4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.71</v>
+        <v>0.6</v>
       </c>
       <c r="R4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="S4">
         <f ca="1">RANDBETWEEN(0,100)/100</f>
-        <v>0.46</v>
+        <v>0.33</v>
       </c>
       <c r="T4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.67</v>
+        <v>0.01</v>
       </c>
       <c r="U4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.83</v>
+        <v>0.42</v>
       </c>
       <c r="V4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.65</v>
+        <v>0.51</v>
       </c>
       <c r="W4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.06</v>
+        <v>0.16</v>
       </c>
       <c r="X4">
         <f t="shared" ca="1" si="0"/>
-        <v>7.0000000000000007E-2</v>
+        <v>0.93</v>
       </c>
       <c r="Y4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.69</v>
+        <v>0.41</v>
       </c>
       <c r="Z4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.88</v>
+        <v>0.62</v>
       </c>
       <c r="AA4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.34</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
@@ -35466,12 +35549,12 @@
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <conditionalFormatting sqref="A4:A36">
-    <cfRule type="containsBlanks" dxfId="9" priority="1">
+    <cfRule type="containsBlanks" dxfId="13" priority="1">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:AA36">
-    <cfRule type="containsBlanks" dxfId="8" priority="2">
+    <cfRule type="containsBlanks" dxfId="12" priority="2">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -35539,18 +35622,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="79" t="s">
         <v>750</v>
       </c>
-      <c r="B1" s="122" t="s">
+      <c r="B1" s="121" t="s">
         <v>753</v>
       </c>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="124"/>
+      <c r="C1" s="122"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="122"/>
+      <c r="F1" s="122"/>
+      <c r="G1" s="122"/>
+      <c r="H1" s="123"/>
     </row>
     <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="50" t="s">
@@ -35574,7 +35657,7 @@
       <c r="G2" s="51" t="s">
         <v>729</v>
       </c>
-      <c r="H2" s="90" t="s">
+      <c r="H2" s="89" t="s">
         <v>730</v>
       </c>
     </row>
@@ -35661,17 +35744,17 @@
     <mergeCell ref="B1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="A3:A43">
-    <cfRule type="containsBlanks" dxfId="7" priority="4">
+    <cfRule type="containsBlanks" dxfId="11" priority="4">
       <formula>LEN(TRIM(A3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:H3 B6:H43">
-    <cfRule type="containsBlanks" dxfId="6" priority="3">
+    <cfRule type="containsBlanks" dxfId="10" priority="3">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:H5">
-    <cfRule type="containsBlanks" dxfId="5" priority="1">
+    <cfRule type="containsBlanks" dxfId="9" priority="1">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -35712,26 +35795,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="79" t="s">
         <v>750</v>
       </c>
-      <c r="B1" s="88" t="s">
+      <c r="B1" s="87" t="s">
         <v>754</v>
       </c>
-      <c r="C1" s="129" t="s">
+      <c r="C1" s="128" t="s">
         <v>753</v>
       </c>
-      <c r="D1" s="130"/>
-      <c r="E1" s="130"/>
-      <c r="F1" s="130"/>
-      <c r="G1" s="130"/>
-      <c r="H1" s="130"/>
-      <c r="I1" s="130"/>
-      <c r="J1" s="130"/>
-      <c r="K1" s="130"/>
-      <c r="L1" s="130"/>
-      <c r="M1" s="130"/>
-      <c r="N1" s="131"/>
+      <c r="D1" s="129"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="129"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="129"/>
+      <c r="J1" s="129"/>
+      <c r="K1" s="129"/>
+      <c r="L1" s="129"/>
+      <c r="M1" s="129"/>
+      <c r="N1" s="130"/>
     </row>
     <row r="2" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="50" t="s">
@@ -35773,7 +35856,7 @@
       <c r="M2" s="51" t="s">
         <v>744</v>
       </c>
-      <c r="N2" s="90" t="s">
+      <c r="N2" s="89" t="s">
         <v>745</v>
       </c>
     </row>
@@ -35854,7 +35937,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="78" t="s">
+      <c r="A8" s="77" t="s">
         <v>802</v>
       </c>
       <c r="B8" t="s">
@@ -35898,7 +35981,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="78" t="s">
+      <c r="A9" s="77" t="s">
         <v>803</v>
       </c>
       <c r="B9" t="s">
@@ -35986,7 +36069,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="78" t="s">
+      <c r="A11" s="77" t="s">
         <v>805</v>
       </c>
       <c r="B11" t="s">
@@ -36030,7 +36113,7 @@
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="78" t="s">
+      <c r="A12" s="77" t="s">
         <v>806</v>
       </c>
       <c r="B12" t="s">
@@ -36046,7 +36129,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="92" t="s">
+      <c r="A14" s="91" t="s">
         <v>808</v>
       </c>
       <c r="B14" t="s">
@@ -36054,7 +36137,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="92" t="s">
+      <c r="A15" s="91" t="s">
         <v>809</v>
       </c>
       <c r="B15" t="s">
@@ -36062,7 +36145,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="77" t="s">
+      <c r="A16" s="76" t="s">
         <v>552</v>
       </c>
       <c r="B16" t="s">
@@ -36070,7 +36153,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="77" t="s">
+      <c r="A17" s="76" t="s">
         <v>553</v>
       </c>
       <c r="B17" t="s">
@@ -36078,7 +36161,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="77" t="s">
+      <c r="A18" s="76" t="s">
         <v>554</v>
       </c>
       <c r="B18" t="s">
@@ -36086,7 +36169,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="77" t="s">
+      <c r="A19" s="76" t="s">
         <v>555</v>
       </c>
       <c r="B19" t="s">
@@ -36094,7 +36177,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="77" t="s">
+      <c r="A20" s="76" t="s">
         <v>556</v>
       </c>
       <c r="B20" t="s">
@@ -36102,7 +36185,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="77" t="s">
+      <c r="A21" s="76" t="s">
         <v>557</v>
       </c>
       <c r="B21" t="s">
@@ -36110,7 +36193,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="77" t="s">
+      <c r="A22" s="76" t="s">
         <v>558</v>
       </c>
       <c r="B22" t="s">
@@ -36118,7 +36201,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="77" t="s">
+      <c r="A23" s="76" t="s">
         <v>559</v>
       </c>
       <c r="B23" t="s">
@@ -36126,7 +36209,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="77" t="s">
+      <c r="A24" s="76" t="s">
         <v>560</v>
       </c>
       <c r="B24" t="s">
@@ -36134,7 +36217,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="77" t="s">
+      <c r="A25" s="76" t="s">
         <v>561</v>
       </c>
       <c r="B25" t="s">
@@ -36142,7 +36225,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="77" t="s">
+      <c r="A26" s="76" t="s">
         <v>552</v>
       </c>
       <c r="B26" t="s">
@@ -36150,7 +36233,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="77" t="s">
+      <c r="A27" s="76" t="s">
         <v>553</v>
       </c>
       <c r="B27" t="s">
@@ -36158,7 +36241,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="77" t="s">
+      <c r="A28" s="76" t="s">
         <v>554</v>
       </c>
       <c r="B28" t="s">
@@ -36166,7 +36249,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="77" t="s">
+      <c r="A29" s="76" t="s">
         <v>555</v>
       </c>
       <c r="B29" t="s">
@@ -36174,7 +36257,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="77" t="s">
+      <c r="A30" s="76" t="s">
         <v>556</v>
       </c>
       <c r="B30" t="s">
@@ -36182,7 +36265,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="77" t="s">
+      <c r="A31" s="76" t="s">
         <v>557</v>
       </c>
       <c r="B31" t="s">
@@ -36190,7 +36273,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="77" t="s">
+      <c r="A32" s="76" t="s">
         <v>558</v>
       </c>
       <c r="B32" t="s">
@@ -36198,7 +36281,7 @@
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A33" s="77" t="s">
+      <c r="A33" s="76" t="s">
         <v>559</v>
       </c>
       <c r="B33" t="s">
@@ -36206,7 +36289,7 @@
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A34" s="77" t="s">
+      <c r="A34" s="76" t="s">
         <v>560</v>
       </c>
       <c r="B34" t="s">
@@ -36214,7 +36297,7 @@
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A35" s="77" t="s">
+      <c r="A35" s="76" t="s">
         <v>561</v>
       </c>
       <c r="B35" t="s">
@@ -36222,7 +36305,7 @@
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A36" s="92" t="s">
+      <c r="A36" s="91" t="s">
         <v>552</v>
       </c>
       <c r="B36" t="s">
@@ -36230,7 +36313,7 @@
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A37" s="92" t="s">
+      <c r="A37" s="91" t="s">
         <v>553</v>
       </c>
       <c r="B37" t="s">
@@ -36238,7 +36321,7 @@
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A38" s="92" t="s">
+      <c r="A38" s="91" t="s">
         <v>554</v>
       </c>
       <c r="B38" t="s">
@@ -36246,7 +36329,7 @@
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A39" s="92" t="s">
+      <c r="A39" s="91" t="s">
         <v>555</v>
       </c>
       <c r="B39" t="s">
@@ -36254,7 +36337,7 @@
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A40" s="92" t="s">
+      <c r="A40" s="91" t="s">
         <v>556</v>
       </c>
       <c r="B40" t="s">
@@ -36262,7 +36345,7 @@
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A41" s="92" t="s">
+      <c r="A41" s="91" t="s">
         <v>557</v>
       </c>
       <c r="B41" t="s">
@@ -36270,7 +36353,7 @@
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A42" s="92" t="s">
+      <c r="A42" s="91" t="s">
         <v>558</v>
       </c>
       <c r="B42" t="s">
@@ -36278,7 +36361,7 @@
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A43" s="92" t="s">
+      <c r="A43" s="91" t="s">
         <v>559</v>
       </c>
       <c r="B43" t="s">
@@ -36286,7 +36369,7 @@
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A44" s="92" t="s">
+      <c r="A44" s="91" t="s">
         <v>560</v>
       </c>
       <c r="B44" t="s">
@@ -36294,7 +36377,7 @@
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A45" s="92" t="s">
+      <c r="A45" s="91" t="s">
         <v>561</v>
       </c>
       <c r="B45" t="s">
@@ -36302,7 +36385,7 @@
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A46" s="92" t="s">
+      <c r="A46" s="91" t="s">
         <v>810</v>
       </c>
       <c r="B46" t="s">
@@ -36346,7 +36429,7 @@
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A47" s="92" t="s">
+      <c r="A47" s="91" t="s">
         <v>811</v>
       </c>
       <c r="B47" t="s">
@@ -36394,22 +36477,22 @@
     <mergeCell ref="C1:N1"/>
   </mergeCells>
   <conditionalFormatting sqref="A3:A35 A46:A49">
-    <cfRule type="containsBlanks" dxfId="4" priority="5">
+    <cfRule type="containsBlanks" dxfId="8" priority="5">
       <formula>LEN(TRIM(A3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:N6 B7:B11 B12:N45 B46:B47 B48:N49">
-    <cfRule type="containsBlanks" dxfId="3" priority="6">
+    <cfRule type="containsBlanks" dxfId="7" priority="6">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:N11">
-    <cfRule type="containsBlanks" dxfId="2" priority="3">
+    <cfRule type="containsBlanks" dxfId="6" priority="3">
       <formula>LEN(TRIM(C7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:N47">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
+    <cfRule type="containsBlanks" dxfId="5" priority="1">
       <formula>LEN(TRIM(C46))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -38047,17 +38130,17 @@
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <conditionalFormatting sqref="A3:A139">
-    <cfRule type="containsBlanks" dxfId="52" priority="1">
+    <cfRule type="containsBlanks" dxfId="56" priority="1">
       <formula>LEN(TRIM(A3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C139">
-    <cfRule type="containsBlanks" dxfId="51" priority="3">
+    <cfRule type="containsBlanks" dxfId="55" priority="3">
       <formula>LEN(TRIM(C3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9:E139">
-    <cfRule type="containsBlanks" dxfId="50" priority="2">
+    <cfRule type="containsBlanks" dxfId="54" priority="2">
       <formula>LEN(TRIM(E9))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -38161,8 +38244,8 @@
       <c r="E1" s="49" t="s">
         <v>518</v>
       </c>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
       <c r="H1" s="49" t="s">
         <v>516</v>
       </c>
@@ -38174,34 +38257,34 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="72" t="s">
         <v>748</v>
       </c>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="72" t="s">
         <v>749</v>
       </c>
-      <c r="C2" s="73" t="s">
+      <c r="C2" s="72" t="s">
         <v>512</v>
       </c>
-      <c r="D2" s="73" t="s">
+      <c r="D2" s="72" t="s">
         <v>470</v>
       </c>
-      <c r="E2" s="73" t="s">
+      <c r="E2" s="72" t="s">
         <v>529</v>
       </c>
-      <c r="F2" s="73" t="s">
+      <c r="F2" s="72" t="s">
         <v>535</v>
       </c>
-      <c r="G2" s="73" t="s">
+      <c r="G2" s="72" t="s">
         <v>531</v>
       </c>
-      <c r="H2" s="73" t="s">
+      <c r="H2" s="72" t="s">
         <v>513</v>
       </c>
-      <c r="I2" s="74" t="s">
+      <c r="I2" s="73" t="s">
         <v>457</v>
       </c>
-      <c r="J2" s="75" t="s">
+      <c r="J2" s="74" t="s">
         <v>456</v>
       </c>
     </row>
@@ -38233,7 +38316,7 @@
       <c r="I3" s="40" t="s">
         <v>546</v>
       </c>
-      <c r="J3" s="72"/>
+      <c r="J3" s="71"/>
     </row>
     <row r="4" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="37" t="s">
@@ -38263,7 +38346,7 @@
       <c r="I4" s="41" t="s">
         <v>460</v>
       </c>
-      <c r="J4" s="72"/>
+      <c r="J4" s="71"/>
     </row>
     <row r="5" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="37" t="s">
@@ -38293,7 +38376,7 @@
       <c r="I5" s="41" t="s">
         <v>462</v>
       </c>
-      <c r="J5" s="72"/>
+      <c r="J5" s="71"/>
     </row>
     <row r="6" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="37" t="s">
@@ -38323,7 +38406,7 @@
       <c r="I6" s="41" t="s">
         <v>464</v>
       </c>
-      <c r="J6" s="72"/>
+      <c r="J6" s="71"/>
     </row>
     <row r="7" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="37" t="s">
@@ -38353,7 +38436,7 @@
       <c r="I7" s="42" t="s">
         <v>465</v>
       </c>
-      <c r="J7" s="72"/>
+      <c r="J7" s="71"/>
     </row>
     <row r="8" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="37" t="s">
@@ -38383,7 +38466,7 @@
       <c r="I8" s="41" t="s">
         <v>466</v>
       </c>
-      <c r="J8" s="72"/>
+      <c r="J8" s="71"/>
     </row>
     <row r="9" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="37" t="s">
@@ -38413,7 +38496,7 @@
       <c r="I9" s="42" t="s">
         <v>467</v>
       </c>
-      <c r="J9" s="72"/>
+      <c r="J9" s="71"/>
     </row>
     <row r="10" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="37" t="s">
@@ -38443,7 +38526,7 @@
       <c r="I10" s="41" t="s">
         <v>469</v>
       </c>
-      <c r="J10" s="72"/>
+      <c r="J10" s="71"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="37" t="s">
@@ -38874,7 +38957,7 @@
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <conditionalFormatting sqref="A11:A14 C11:J14 A15:J71">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="4" priority="1">
       <formula>LEN(TRIM(A11))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -38926,12 +39009,12 @@
         <v>516</v>
       </c>
       <c r="B1" s="70"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
-      <c r="G1" s="126"/>
-      <c r="H1" s="126"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="125"/>
+      <c r="E1" s="125"/>
+      <c r="F1" s="125"/>
+      <c r="G1" s="125"/>
+      <c r="H1" s="125"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="43" t="s">
@@ -38946,7 +39029,7 @@
       <c r="D2" s="43" t="s">
         <v>783</v>
       </c>
-      <c r="E2" s="102"/>
+      <c r="E2" s="101"/>
       <c r="F2" s="43"/>
       <c r="G2" s="43"/>
       <c r="H2" s="45"/>
@@ -39570,13 +39653,13 @@
       <c r="K2" s="50" t="s">
         <v>578</v>
       </c>
-      <c r="L2" s="79" t="s">
+      <c r="L2" s="78" t="s">
         <v>572</v>
       </c>
-      <c r="M2" s="79" t="s">
+      <c r="M2" s="78" t="s">
         <v>590</v>
       </c>
-      <c r="N2" s="79" t="s">
+      <c r="N2" s="78" t="s">
         <v>591</v>
       </c>
     </row>
@@ -40188,7 +40271,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="76" t="s">
         <v>551</v>
       </c>
       <c r="B3" t="str">
@@ -40206,7 +40289,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="77" t="s">
         <v>603</v>
       </c>
       <c r="B4" t="str">
@@ -40223,7 +40306,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="77" t="s">
+      <c r="A5" s="76" t="s">
         <v>552</v>
       </c>
       <c r="B5" t="str">
@@ -40240,7 +40323,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="77" t="s">
+      <c r="A6" s="76" t="s">
         <v>553</v>
       </c>
       <c r="B6" t="str">
@@ -40254,7 +40337,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="77" t="s">
+      <c r="A7" s="76" t="s">
         <v>554</v>
       </c>
       <c r="B7" t="str">
@@ -40268,7 +40351,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="77" t="s">
+      <c r="A8" s="76" t="s">
         <v>555</v>
       </c>
       <c r="B8" t="str">
@@ -40282,7 +40365,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="77" t="s">
+      <c r="A9" s="76" t="s">
         <v>556</v>
       </c>
       <c r="B9" t="str">
@@ -40296,7 +40379,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="77" t="s">
+      <c r="A10" s="76" t="s">
         <v>557</v>
       </c>
       <c r="B10" t="str">
@@ -40310,7 +40393,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="77" t="s">
+      <c r="A11" s="76" t="s">
         <v>558</v>
       </c>
       <c r="B11" t="str">
@@ -40324,7 +40407,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="77" t="s">
+      <c r="A12" s="76" t="s">
         <v>559</v>
       </c>
       <c r="B12" t="str">
@@ -40338,7 +40421,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="77" t="s">
+      <c r="A13" s="76" t="s">
         <v>560</v>
       </c>
       <c r="B13" t="str">
@@ -40352,7 +40435,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="77" t="s">
+      <c r="A14" s="76" t="s">
         <v>561</v>
       </c>
       <c r="B14" t="str">
@@ -40575,10 +40658,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="79" t="s">
         <v>793</v>
       </c>
-      <c r="B1" s="88" t="s">
+      <c r="B1" s="87" t="s">
         <v>794</v>
       </c>
     </row>
@@ -41394,12 +41477,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A49">
-    <cfRule type="containsBlanks" dxfId="49" priority="2">
+    <cfRule type="containsBlanks" dxfId="53" priority="2">
       <formula>LEN(TRIM(A3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C49 E3:E49">
-    <cfRule type="containsBlanks" dxfId="48" priority="3">
+    <cfRule type="containsBlanks" dxfId="52" priority="3">
       <formula>LEN(TRIM(C3))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41435,20 +41518,20 @@
     <col min="1" max="2" width="43.83203125" customWidth="1"/>
     <col min="3" max="3" width="43.83203125" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="43.83203125" customWidth="1"/>
-    <col min="5" max="5" width="43.83203125" style="99" customWidth="1"/>
+    <col min="5" max="5" width="43.83203125" style="98" customWidth="1"/>
     <col min="6" max="6" width="18.83203125" style="5" customWidth="1"/>
     <col min="7" max="16384" width="8.83203125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="79" t="s">
         <v>453</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="99" t="s">
         <v>826</v>
       </c>
-      <c r="C1" s="103"/>
-      <c r="E1" s="100" t="s">
+      <c r="C1" s="102"/>
+      <c r="E1" s="99" t="s">
         <v>825</v>
       </c>
     </row>
@@ -41459,16 +41542,16 @@
       <c r="B2" s="51" t="s">
         <v>373</v>
       </c>
-      <c r="C2" s="104" t="s">
+      <c r="C2" s="103" t="s">
         <v>891</v>
       </c>
       <c r="D2" s="51" t="s">
         <v>684</v>
       </c>
-      <c r="E2" s="98" t="s">
+      <c r="E2" s="97" t="s">
         <v>566</v>
       </c>
-      <c r="F2" s="98" t="s">
+      <c r="F2" s="97" t="s">
         <v>844</v>
       </c>
     </row>
@@ -41775,17 +41858,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:E4">
-    <cfRule type="containsBlanks" dxfId="47" priority="1">
+    <cfRule type="containsBlanks" dxfId="51" priority="1">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:E55">
-    <cfRule type="containsBlanks" dxfId="46" priority="4">
+    <cfRule type="containsBlanks" dxfId="50" priority="4">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:E55">
-    <cfRule type="containsBlanks" dxfId="45" priority="3">
+    <cfRule type="containsBlanks" dxfId="49" priority="3">
       <formula>LEN(TRIM(E5))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41826,14 +41909,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="79" t="s">
         <v>453</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="99" t="s">
         <v>827</v>
       </c>
-      <c r="C1" s="103"/>
-      <c r="E1" s="100" t="s">
+      <c r="C1" s="102"/>
+      <c r="E1" s="99" t="s">
         <v>828</v>
       </c>
     </row>
@@ -41850,7 +41933,7 @@
       <c r="D2" s="54" t="s">
         <v>569</v>
       </c>
-      <c r="E2" s="81" t="s">
+      <c r="E2" s="80" t="s">
         <v>686</v>
       </c>
     </row>
@@ -42169,17 +42252,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:E6">
-    <cfRule type="containsBlanks" dxfId="44" priority="1">
+    <cfRule type="containsBlanks" dxfId="48" priority="1">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:E55">
-    <cfRule type="containsBlanks" dxfId="43" priority="3">
+    <cfRule type="containsBlanks" dxfId="47" priority="3">
       <formula>LEN(TRIM(B7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:D55">
-    <cfRule type="containsBlanks" dxfId="42" priority="2">
+    <cfRule type="containsBlanks" dxfId="46" priority="2">
       <formula>LEN(TRIM(D7))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update the construction types
</commit_message>
<xml_diff>
--- a/tests/data/template_tester_v3.xlsx
+++ b/tests/data/template_tester_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daryaguettler/MIT Dropbox/Darya Guettler/Research/epinterface/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FFC641-B4D4-F441-B943-C20EC015D6FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380CD583-7837-A349-BD4F-96BA8A65EA51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16680" tabRatio="926" firstSheet="14" activeTab="22" xr2:uid="{46D55ACF-0183-F346-B7C2-C9B3BC712B05}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16680" tabRatio="926" firstSheet="14" activeTab="23" xr2:uid="{46D55ACF-0183-F346-B7C2-C9B3BC712B05}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -4119,7 +4119,28 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="58">
+  <dxfs count="59">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -6218,7 +6239,7 @@
     <mergeCell ref="A11:A12"/>
   </mergeCells>
   <conditionalFormatting sqref="G20">
-    <cfRule type="containsBlanks" dxfId="57" priority="1">
+    <cfRule type="containsBlanks" dxfId="58" priority="1">
       <formula>LEN(TRIM(G20))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6599,12 +6620,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:D3 D4:D57 B4:C55">
-    <cfRule type="containsBlanks" dxfId="44" priority="2">
+    <cfRule type="containsBlanks" dxfId="45" priority="2">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D57">
-    <cfRule type="containsBlanks" dxfId="43" priority="1">
+    <cfRule type="containsBlanks" dxfId="44" priority="1">
       <formula>LEN(TRIM(D3))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6736,30 +6757,30 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:B55">
-    <cfRule type="containsBlanks" dxfId="42" priority="5">
+    <cfRule type="containsBlanks" dxfId="43" priority="5">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:C55">
-    <cfRule type="containsBlanks" dxfId="41" priority="6">
+    <cfRule type="containsBlanks" dxfId="42" priority="6">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D55">
-    <cfRule type="containsBlanks" dxfId="40" priority="3">
+    <cfRule type="containsBlanks" dxfId="41" priority="3">
       <formula>LEN(TRIM(D3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:E55">
-    <cfRule type="containsBlanks" dxfId="39" priority="4">
+    <cfRule type="containsBlanks" dxfId="40" priority="4">
       <formula>LEN(TRIM(D3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:G55">
-    <cfRule type="containsBlanks" dxfId="38" priority="1">
+    <cfRule type="containsBlanks" dxfId="39" priority="1">
       <formula>LEN(TRIM(F3))=0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="37" priority="2">
+    <cfRule type="containsBlanks" dxfId="38" priority="2">
       <formula>LEN(TRIM(F3))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7113,17 +7134,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:D55">
-    <cfRule type="containsBlanks" dxfId="36" priority="2">
+    <cfRule type="containsBlanks" dxfId="37" priority="2">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B307:D1048576">
-    <cfRule type="containsBlanks" dxfId="35" priority="3">
+    <cfRule type="containsBlanks" dxfId="36" priority="3">
       <formula>LEN(TRIM(B307))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="containsBlanks" dxfId="34" priority="1">
+    <cfRule type="containsBlanks" dxfId="35" priority="1">
       <formula>LEN(TRIM(C3))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7238,10 +7259,10 @@
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <conditionalFormatting sqref="B3:F55">
-    <cfRule type="containsBlanks" dxfId="33" priority="1">
+    <cfRule type="containsBlanks" dxfId="34" priority="1">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="32" priority="2">
+    <cfRule type="containsBlanks" dxfId="33" priority="2">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8018,15 +8039,15 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:F57">
-    <cfRule type="containsBlanks" dxfId="31" priority="3">
+    <cfRule type="containsBlanks" dxfId="32" priority="3">
       <formula>LEN(TRIM(A3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:D57">
-    <cfRule type="containsBlanks" dxfId="30" priority="1">
+    <cfRule type="containsBlanks" dxfId="31" priority="1">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="29" priority="4" stopIfTrue="1">
+    <cfRule type="containsBlanks" dxfId="30" priority="4" stopIfTrue="1">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9270,17 +9291,17 @@
     <mergeCell ref="C1:J1"/>
   </mergeCells>
   <conditionalFormatting sqref="A3:F3 H4:I124 E7:J121 A4:C121 D4:D208 E4:F6 F3:F6">
-    <cfRule type="containsBlanks" dxfId="28" priority="4">
+    <cfRule type="containsBlanks" dxfId="29" priority="4">
       <formula>LEN(TRIM(A3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:J124">
-    <cfRule type="containsBlanks" dxfId="27" priority="1">
+    <cfRule type="containsBlanks" dxfId="28" priority="1">
       <formula>LEN(TRIM(E3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:J6">
-    <cfRule type="containsBlanks" dxfId="26" priority="2">
+    <cfRule type="containsBlanks" dxfId="27" priority="2">
       <formula>LEN(TRIM(G3))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9648,7 +9669,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A116 C3:C116 E3:E116">
-    <cfRule type="containsBlanks" dxfId="25" priority="1">
+    <cfRule type="containsBlanks" dxfId="26" priority="1">
       <formula>LEN(TRIM(A3))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9808,17 +9829,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:F143">
-    <cfRule type="containsBlanks" dxfId="24" priority="4">
+    <cfRule type="containsBlanks" dxfId="25" priority="4">
       <formula>LEN(TRIM(A3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B143">
-    <cfRule type="containsBlanks" dxfId="23" priority="3">
+    <cfRule type="containsBlanks" dxfId="24" priority="3">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="containsBlanks" dxfId="22" priority="2">
+    <cfRule type="containsBlanks" dxfId="23" priority="2">
       <formula>LEN(TRIM(F2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10557,7 +10578,7 @@
     <mergeCell ref="C8:J8"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:B9">
-    <cfRule type="containsBlanks" dxfId="56" priority="1">
+    <cfRule type="containsBlanks" dxfId="57" priority="1">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -28978,9 +28999,9 @@
   </sheetPr>
   <dimension ref="A1:CF89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -33616,32 +33637,32 @@
     <mergeCell ref="F1:M1"/>
   </mergeCells>
   <conditionalFormatting sqref="A6:B83 R6:R83">
-    <cfRule type="containsBlanks" dxfId="21" priority="9">
+    <cfRule type="containsBlanks" dxfId="22" priority="9">
       <formula>LEN(TRIM(A6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B83">
-    <cfRule type="containsBlanks" dxfId="20" priority="5">
+    <cfRule type="containsBlanks" dxfId="21" priority="5">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10 H10 J10:J74 H12:H74 F12:F74">
-    <cfRule type="containsBlanks" dxfId="19" priority="4">
+    <cfRule type="containsBlanks" dxfId="20" priority="4">
       <formula>LEN(TRIM(F10))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9:L74">
-    <cfRule type="containsBlanks" dxfId="18" priority="3">
+    <cfRule type="containsBlanks" dxfId="19" priority="3">
       <formula>LEN(TRIM(L9))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N9:N74">
-    <cfRule type="containsBlanks" dxfId="17" priority="2">
+    <cfRule type="containsBlanks" dxfId="18" priority="2">
       <formula>LEN(TRIM(N9))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P9:P74">
-    <cfRule type="containsBlanks" dxfId="16" priority="1">
+    <cfRule type="containsBlanks" dxfId="17" priority="1">
       <formula>LEN(TRIM(P9))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33674,11 +33695,11 @@
   </sheetPr>
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
       <pane xSplit="12" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomRight" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -33825,7 +33846,7 @@
         <v>901</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>344</v>
+        <v>902</v>
       </c>
       <c r="K4" t="s">
         <v>902</v>
@@ -33842,28 +33863,33 @@
     <mergeCell ref="G1:M1"/>
   </mergeCells>
   <conditionalFormatting sqref="A5:M91 A4:E4">
-    <cfRule type="containsBlanks" dxfId="15" priority="5">
+    <cfRule type="containsBlanks" dxfId="16" priority="6">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I4">
-    <cfRule type="containsBlanks" dxfId="14" priority="4">
+    <cfRule type="containsBlanks" dxfId="15" priority="5">
       <formula>LEN(TRIM(I3))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K4">
-    <cfRule type="containsBlanks" dxfId="13" priority="3">
+  <conditionalFormatting sqref="K3">
+    <cfRule type="containsBlanks" dxfId="14" priority="4">
       <formula>LEN(TRIM(K3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:L4">
-    <cfRule type="containsBlanks" dxfId="12" priority="2">
+    <cfRule type="containsBlanks" dxfId="13" priority="3">
       <formula>LEN(TRIM(L3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3:M4">
-    <cfRule type="containsBlanks" dxfId="11" priority="1">
+    <cfRule type="containsBlanks" dxfId="12" priority="2">
       <formula>LEN(TRIM(M3))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(K4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -34060,7 +34086,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B4">
-    <cfRule type="containsBlanks" dxfId="10" priority="1">
+    <cfRule type="containsBlanks" dxfId="11" priority="1">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -34296,103 +34322,103 @@
       </c>
       <c r="C4">
         <f ca="1">RANDBETWEEN(0,100)/100</f>
-        <v>0.31</v>
+        <v>0.86</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:AA4" ca="1" si="0">RANDBETWEEN(0,100)/100</f>
-        <v>0.21</v>
+        <v>0.97</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11</v>
+        <v>0.51</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.14000000000000001</v>
+        <v>0.79</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.7</v>
+        <v>0.11</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.64</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.92</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.24</v>
+        <v>0.19</v>
       </c>
       <c r="L4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.88</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="M4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.31</v>
+        <v>0.76</v>
       </c>
       <c r="N4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.37</v>
+        <v>0</v>
       </c>
       <c r="O4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.23</v>
+        <v>0.5</v>
       </c>
       <c r="P4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.63</v>
+        <v>0.99</v>
       </c>
       <c r="Q4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.86</v>
+        <v>0.97</v>
       </c>
       <c r="R4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.97</v>
+        <v>0.5</v>
       </c>
       <c r="S4">
         <f ca="1">RANDBETWEEN(0,100)/100</f>
-        <v>0.37</v>
+        <v>0.19</v>
       </c>
       <c r="T4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.48</v>
+        <v>0.16</v>
       </c>
       <c r="U4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.13</v>
+        <v>0.74</v>
       </c>
       <c r="V4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.38</v>
+        <v>0.01</v>
       </c>
       <c r="W4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.3</v>
+        <v>0.24</v>
       </c>
       <c r="X4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.02</v>
+        <v>0.33</v>
       </c>
       <c r="Y4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.83</v>
+        <v>0.53</v>
       </c>
       <c r="Z4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.88</v>
+        <v>0.02</v>
       </c>
       <c r="AA4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.9</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
@@ -34717,12 +34743,12 @@
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <conditionalFormatting sqref="A4:A36">
-    <cfRule type="containsBlanks" dxfId="9" priority="1">
+    <cfRule type="containsBlanks" dxfId="10" priority="1">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:AA36">
-    <cfRule type="containsBlanks" dxfId="8" priority="2">
+    <cfRule type="containsBlanks" dxfId="9" priority="2">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -34912,17 +34938,17 @@
     <mergeCell ref="B1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="A3:A43">
-    <cfRule type="containsBlanks" dxfId="7" priority="4">
+    <cfRule type="containsBlanks" dxfId="8" priority="4">
       <formula>LEN(TRIM(A3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:H3 B6:H43">
-    <cfRule type="containsBlanks" dxfId="6" priority="3">
+    <cfRule type="containsBlanks" dxfId="7" priority="3">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:H5">
-    <cfRule type="containsBlanks" dxfId="5" priority="1">
+    <cfRule type="containsBlanks" dxfId="6" priority="1">
       <formula>LEN(TRIM(B4))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -35645,22 +35671,22 @@
     <mergeCell ref="C1:N1"/>
   </mergeCells>
   <conditionalFormatting sqref="A3:A35 A46:A49">
-    <cfRule type="containsBlanks" dxfId="4" priority="5">
+    <cfRule type="containsBlanks" dxfId="5" priority="5">
       <formula>LEN(TRIM(A3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:N6 B7:B11 B12:N45 B46:B47 B48:N49">
-    <cfRule type="containsBlanks" dxfId="3" priority="6">
+    <cfRule type="containsBlanks" dxfId="4" priority="6">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:N11">
-    <cfRule type="containsBlanks" dxfId="2" priority="3">
+    <cfRule type="containsBlanks" dxfId="3" priority="3">
       <formula>LEN(TRIM(C7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46:N47">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
+    <cfRule type="containsBlanks" dxfId="2" priority="1">
       <formula>LEN(TRIM(C46))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -37298,17 +37324,17 @@
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <conditionalFormatting sqref="A3:A139">
-    <cfRule type="containsBlanks" dxfId="55" priority="1">
+    <cfRule type="containsBlanks" dxfId="56" priority="1">
       <formula>LEN(TRIM(A3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C139">
-    <cfRule type="containsBlanks" dxfId="54" priority="3">
+    <cfRule type="containsBlanks" dxfId="55" priority="3">
       <formula>LEN(TRIM(C3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9:E139">
-    <cfRule type="containsBlanks" dxfId="53" priority="2">
+    <cfRule type="containsBlanks" dxfId="54" priority="2">
       <formula>LEN(TRIM(E9))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -38125,7 +38151,7 @@
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <conditionalFormatting sqref="A11:A14 C11:J14 A15:J71">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(A11))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -40610,12 +40636,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A49">
-    <cfRule type="containsBlanks" dxfId="52" priority="2">
+    <cfRule type="containsBlanks" dxfId="53" priority="2">
       <formula>LEN(TRIM(A3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C49 E3:E49">
-    <cfRule type="containsBlanks" dxfId="51" priority="3">
+    <cfRule type="containsBlanks" dxfId="52" priority="3">
       <formula>LEN(TRIM(C3))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -40991,17 +41017,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:E4">
-    <cfRule type="containsBlanks" dxfId="50" priority="1">
+    <cfRule type="containsBlanks" dxfId="51" priority="1">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:E55">
-    <cfRule type="containsBlanks" dxfId="49" priority="4">
+    <cfRule type="containsBlanks" dxfId="50" priority="4">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:E55">
-    <cfRule type="containsBlanks" dxfId="48" priority="3">
+    <cfRule type="containsBlanks" dxfId="49" priority="3">
       <formula>LEN(TRIM(E5))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41385,17 +41411,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:E6">
-    <cfRule type="containsBlanks" dxfId="47" priority="1">
+    <cfRule type="containsBlanks" dxfId="48" priority="1">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:E55">
-    <cfRule type="containsBlanks" dxfId="46" priority="3">
+    <cfRule type="containsBlanks" dxfId="47" priority="3">
       <formula>LEN(TRIM(B7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:D55">
-    <cfRule type="containsBlanks" dxfId="45" priority="2">
+    <cfRule type="containsBlanks" dxfId="46" priority="2">
       <formula>LEN(TRIM(D7))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>